<commit_message>
implement master mix distribution, update messages
</commit_message>
<xml_diff>
--- a/templates/01-sanger-master-v3.xlsx
+++ b/templates/01-sanger-master-v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelangelov/code/opentrons/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CB553D-31F9-9446-994E-0E09207F4E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83219259-7F23-E043-A8EA-27ACC5CB39F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="192">
   <si>
     <t>source_well</t>
   </si>
@@ -804,6 +804,24 @@
   <dxfs count="4">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -831,24 +849,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -887,7 +887,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E4A5EE2-1080-B34A-BB40-8F3F3FEA7305}" name="Table4" displayName="Table4" ref="A1:B24" totalsRowShown="0">
   <autoFilter ref="A1:B24" xr:uid="{4E4A5EE2-1080-B34A-BB40-8F3F3FEA7305}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CDB38DFA-789C-8F4B-840F-972D89DD6C8F}" name="pos" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{CDB38DFA-789C-8F4B-840F-972D89DD6C8F}" name="pos" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{13A22DA2-122E-D84B-A12E-BE492FE435E8}" name="primer"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1208,7 +1208,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34:C34"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="N7" s="16">
         <f>COUNTIF(K2:K97,"&gt;0")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P7" s="16">
         <f t="shared" si="0"/>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="N8" s="16">
         <f>N7*5.5</f>
-        <v>44</v>
+        <v>60.5</v>
       </c>
       <c r="P8" s="16">
         <f t="shared" si="0"/>
@@ -1695,6 +1695,12 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B10" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="7" t="str">
         <f>IF(F10="","", INDEX(Table4[],MATCH(F10,Table4[primer],0),1))</f>
         <v/>
@@ -1708,11 +1714,11 @@
       </c>
       <c r="K10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="16">
         <f t="shared" si="3"/>
@@ -1720,7 +1726,7 @@
       </c>
       <c r="R10" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T10" s="16" t="s">
         <v>11</v>
@@ -1990,7 +1996,7 @@
       <c r="AE16" s="18"/>
       <c r="AF16" s="18"/>
     </row>
-    <row r="17" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H17" s="7" t="str">
         <f>IF(F17="","", INDEX(Table4[],MATCH(F17,Table4[primer],0),1))</f>
         <v/>
@@ -2037,7 +2043,13 @@
       <c r="AE17" s="18"/>
       <c r="AF17" s="18"/>
     </row>
-    <row r="18" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B18" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="H18" s="7" t="str">
         <f>IF(F18="","", INDEX(Table4[],MATCH(F18,Table4[primer],0),1))</f>
         <v/>
@@ -2051,11 +2063,11 @@
       </c>
       <c r="K18" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P18" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="16">
         <f t="shared" si="3"/>
@@ -2063,7 +2075,7 @@
       </c>
       <c r="R18" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T18" s="18" t="s">
         <v>19</v>
@@ -2084,7 +2096,7 @@
       <c r="AE18" s="18"/>
       <c r="AF18" s="18"/>
     </row>
-    <row r="19" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H19" s="7" t="str">
         <f>IF(F19="","", INDEX(Table4[],MATCH(F19,Table4[primer],0),1))</f>
         <v/>
@@ -2120,7 +2132,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H20" s="7" t="str">
         <f>IF(F20="","", INDEX(Table4[],MATCH(F20,Table4[primer],0),1))</f>
         <v/>
@@ -2156,7 +2168,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H21" s="7" t="str">
         <f>IF(F21="","", INDEX(Table4[],MATCH(F21,Table4[primer],0),1))</f>
         <v/>
@@ -2192,7 +2204,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H22" s="7" t="str">
         <f>IF(F22="","", INDEX(Table4[],MATCH(F22,Table4[primer],0),1))</f>
         <v/>
@@ -2228,7 +2240,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H23" s="7" t="str">
         <f>IF(F23="","", INDEX(Table4[],MATCH(F23,Table4[primer],0),1))</f>
         <v/>
@@ -2264,7 +2276,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H24" s="7" t="str">
         <f>IF(F24="","", INDEX(Table4[],MATCH(F24,Table4[primer],0),1))</f>
         <v/>
@@ -2300,7 +2312,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H25" s="7" t="str">
         <f>IF(F25="","", INDEX(Table4[],MATCH(F25,Table4[primer],0),1))</f>
         <v/>
@@ -2336,7 +2348,13 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B26" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="H26" s="7" t="str">
         <f>IF(F26="","", INDEX(Table4[],MATCH(F26,Table4[primer],0),1))</f>
         <v/>
@@ -2350,11 +2368,11 @@
       </c>
       <c r="K26" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P26" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="16">
         <f t="shared" si="3"/>
@@ -2362,7 +2380,7 @@
       </c>
       <c r="R26" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T26" s="16" t="s">
         <v>27</v>
@@ -2372,7 +2390,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H27" s="7" t="str">
         <f>IF(F27="","", INDEX(Table4[],MATCH(F27,Table4[primer],0),1))</f>
         <v/>
@@ -2408,7 +2426,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H28" s="7" t="str">
         <f>IF(F28="","", INDEX(Table4[],MATCH(F28,Table4[primer],0),1))</f>
         <v/>
@@ -2444,7 +2462,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H29" s="7" t="str">
         <f>IF(F29="","", INDEX(Table4[],MATCH(F29,Table4[primer],0),1))</f>
         <v/>
@@ -2480,7 +2498,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H30" s="7" t="str">
         <f>IF(F30="","", INDEX(Table4[],MATCH(F30,Table4[primer],0),1))</f>
         <v/>
@@ -2516,7 +2534,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H31" s="7" t="str">
         <f>IF(F31="","", INDEX(Table4[],MATCH(F31,Table4[primer],0),1))</f>
         <v/>
@@ -2552,7 +2570,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="8:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
       <c r="H32" s="7" t="str">
         <f>IF(F32="","", INDEX(Table4[],MATCH(F32,Table4[primer],0),1))</f>
         <v/>
@@ -4931,17 +4949,17 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="P2:P97">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q97">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:S97">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
       <formula>1</formula>
       <formula>14</formula>
     </cfRule>
@@ -5897,14 +5915,14 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>IF(master!B10="plate",master!C10, "")</f>
-        <v/>
+        <v>B02</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1">
         <f>IF(master!B10="plate",master!K10,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -6001,14 +6019,14 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(master!B18="plate",master!C18, "")</f>
-        <v/>
+        <v>C03</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1">
         <f>IF(master!B18="plate",master!K18,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -7392,14 +7410,14 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
         <f>IF(master!B26="strip",master!C26,"")</f>
-        <v/>
+        <v>A02</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="1">
         <f>IF(master!B26="strip",master!K26,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -9978,7 +9996,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>source_plate!A10</f>
-        <v/>
+        <v>B02</v>
       </c>
       <c r="B10" t="str">
         <f>source_plate!B10</f>
@@ -9986,7 +10004,7 @@
       </c>
       <c r="C10">
         <f>source_plate!C10</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D10" t="str">
         <f>source_strip!A10</f>
@@ -10282,7 +10300,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>source_plate!A18</f>
-        <v/>
+        <v>C03</v>
       </c>
       <c r="B18" t="str">
         <f>source_plate!B18</f>
@@ -10290,7 +10308,7 @@
       </c>
       <c r="C18">
         <f>source_plate!C18</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D18" t="str">
         <f>source_strip!A18</f>
@@ -10598,7 +10616,7 @@
       </c>
       <c r="D26" t="str">
         <f>source_strip!A26</f>
-        <v/>
+        <v>A02</v>
       </c>
       <c r="E26" t="str">
         <f>source_strip!B26</f>
@@ -10606,7 +10624,7 @@
       </c>
       <c r="F26">
         <f>source_strip!C26</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G26" t="str">
         <f>source_tube!A26</f>
@@ -13326,6 +13344,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FDAF843F15E65A4EA1FFB0CF193B74E3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd4433bf6f24a726161ac457e21002bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1a61fc9-c776-4dd1-85b5-f7d58768ba79" xmlns:ns4="3f421247-72bc-4b61-a591-0b56f96ae993" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d66d7a13b7b51360e8b1c095fb39c19" ns3:_="" ns4:_="">
     <xsd:import namespace="e1a61fc9-c776-4dd1-85b5-f7d58768ba79"/>
@@ -13554,36 +13587,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E774FF9-2144-4DC7-8F36-E7E064C7C739}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79D86924-57C1-45D5-9E44-D526494DB02F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e1a61fc9-c776-4dd1-85b5-f7d58768ba79"/>
-    <ds:schemaRef ds:uri="3f421247-72bc-4b61-a591-0b56f96ae993"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13606,9 +13613,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79D86924-57C1-45D5-9E44-D526494DB02F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E774FF9-2144-4DC7-8F36-E7E064C7C739}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e1a61fc9-c776-4dd1-85b5-f7d58768ba79"/>
+    <ds:schemaRef ds:uri="3f421247-72bc-4b61-a591-0b56f96ae993"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
implemented full column transfer
</commit_message>
<xml_diff>
--- a/templates/01-sanger-master-v3.xlsx
+++ b/templates/01-sanger-master-v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83219259-7F23-E043-A8EA-27ACC5CB39F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB42C825-8B0A-834E-92E8-76FE7935A5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="192">
   <si>
     <t>source_well</t>
   </si>
@@ -583,9 +583,6 @@
     <t>PC pipetting</t>
   </si>
   <si>
-    <t>Positive control</t>
-  </si>
-  <si>
     <t>ready to use premix of pGEM and primer is used, 3.5 ul premix (put it in source_strip) and 11.5 water</t>
   </si>
   <si>
@@ -638,6 +635,9 @@
   </si>
   <si>
     <t>BigDye vol</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -792,11 +792,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,39 +1201,36 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:AF97"/>
+  <dimension ref="A1:U97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="16" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="16"/>
-    <col min="4" max="4" width="13.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="15" style="16" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="16" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="16"/>
-    <col min="12" max="12" width="7.1640625" style="16" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" style="16" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="3.6640625" style="16" customWidth="1"/>
-    <col min="16" max="17" width="11.5" style="16" customWidth="1"/>
-    <col min="18" max="18" width="13" style="16" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" style="18" customWidth="1"/>
-    <col min="20" max="20" width="5.5" style="16" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" style="16" customWidth="1"/>
-    <col min="22" max="32" width="12.83203125" style="16" customWidth="1"/>
-    <col min="33" max="16384" width="10.83203125" style="16"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="3.6640625" customWidth="1"/>
+    <col min="16" max="17" width="11.5" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" customWidth="1"/>
+    <col min="20" max="20" width="5.5" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" customWidth="1"/>
+    <col min="22" max="32" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="11" t="s">
         <v>101</v>
@@ -1264,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
@@ -1277,78 +1271,75 @@
         <v>170</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S1" s="12"/>
       <c r="T1" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="U1" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="U1" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>162</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>105</v>
       </c>
       <c r="H2" s="7" t="str">
         <f>IF(F2="","", INDEX(Table4[],MATCH(F2,Table4[primer],0),1))</f>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="I2" s="7" cm="1">
         <f t="array" ref="I2">_xlfn.IFS(F2="",0,F2="water",11.5, TRUE, 5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="7">
         <f>IF(OR(C2 = "",B2=""),0,15-I2)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2">
         <f t="shared" ref="P2:P33" si="0">COUNTIFS($C$2:$C$97,C2,$B$2:$B$97,B2)</f>
         <v>1</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2">
         <f>COUNTIFS($E$2:$E$97, E2, $F$2:$F$97, F2)</f>
         <v>0</v>
       </c>
-      <c r="R2" s="16">
+      <c r="R2">
         <f t="shared" ref="R2:R66" si="1">I2+K2</f>
         <v>15</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="16" t="str">
+      <c r="U2" t="str">
         <f>TEXT(D2,"")</f>
         <v>Ctf full 2</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" t="s">
         <v>165</v>
       </c>
       <c r="H3" s="7" t="str">
@@ -1369,88 +1360,85 @@
       <c r="M3" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3">
         <f t="shared" ref="Q3:Q33" si="3">COUNTIFS($E$2:$E$97, E3, $F$2:$F$97, F3)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="16" t="str">
+      <c r="U3" t="str">
         <f t="shared" ref="U3:U66" si="4">TEXT(D3,"")</f>
         <v>Ctf full 2</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>162</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>105</v>
       </c>
       <c r="H4" s="7" t="str">
         <f>IF(F4="","", INDEX(Table4[],MATCH(F4,Table4[primer],0),1))</f>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="I4" s="7" cm="1">
         <f t="array" ref="I4">_xlfn.IFS(F4="",0,F4="water",11.5, TRUE, 5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T4" s="16" t="s">
+      <c r="T4" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="16" t="str">
+      <c r="U4" t="str">
         <f t="shared" si="4"/>
         <v>Ctf full 2</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>162</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" t="s">
         <v>164</v>
       </c>
       <c r="H5" s="7" t="str">
@@ -1468,37 +1456,37 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="M5" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="P5" s="16">
+      <c r="M5" t="s">
+        <v>173</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R5" s="16">
+      <c r="R5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T5" s="16" t="s">
+      <c r="T5" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="16" t="str">
+      <c r="U5" t="str">
         <f t="shared" si="4"/>
         <v>Ctf full 2</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>162</v>
       </c>
       <c r="H6" s="7" t="str">
@@ -1516,191 +1504,176 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="P6" s="16">
+      <c r="P6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R6" s="16">
+      <c r="R6">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T6" s="16" t="s">
+      <c r="T6" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="16" t="str">
+      <c r="U6" t="str">
         <f t="shared" si="4"/>
         <v>Ctf full 2</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="16" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>162</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>109</v>
       </c>
       <c r="H7" s="7" t="str">
         <f>IF(F7="","", INDEX(Table4[],MATCH(F7,Table4[primer],0),1))</f>
-        <v>C02</v>
+        <v/>
       </c>
       <c r="I7" s="7" cm="1">
         <f t="array" ref="I7">_xlfn.IFS(F7="",0,F7="water",11.5, TRUE, 5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="N7" s="16">
+        <v>189</v>
+      </c>
+      <c r="N7">
         <f>COUNTIF(K2:K97,"&gt;0")</f>
-        <v>11</v>
-      </c>
-      <c r="P7" s="16">
+        <v>18</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T7" s="16" t="s">
+      <c r="T7" t="s">
         <v>8</v>
       </c>
-      <c r="U7" s="16" t="str">
+      <c r="U7" t="str">
         <f t="shared" si="4"/>
         <v>Ctf full 2</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>171</v>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>191</v>
       </c>
       <c r="H8" s="7" t="str">
         <f>IF(F8="","", INDEX(Table4[],MATCH(F8,Table4[primer],0),1))</f>
-        <v>D05</v>
+        <v/>
       </c>
       <c r="I8" s="7" cm="1">
         <f t="array" ref="I8">_xlfn.IFS(F8="",0,F8="water",11.5, TRUE, 5)</f>
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>15</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="N8" s="16">
-        <f>N7*5.5</f>
-        <v>60.5</v>
-      </c>
-      <c r="P8" s="16">
+        <v>190</v>
+      </c>
+      <c r="N8">
+        <f>N7*5.5*1.1</f>
+        <v>108.9</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Q8" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q8">
         <f>COUNTIFS($E$2:$E$97, E8, $F$2:$F$97, F8)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="16">
+      <c r="R8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T8" s="16" t="s">
+      <c r="T8" t="s">
         <v>9</v>
       </c>
-      <c r="U8" s="16" t="str">
+      <c r="U8" t="str">
         <f t="shared" si="4"/>
-        <v>Positive control</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>171</v>
+        <v>test</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>191</v>
       </c>
       <c r="H9" s="7" t="str">
         <f>IF(F9="","", INDEX(Table4[],MATCH(F9,Table4[primer],0),1))</f>
-        <v>D05</v>
+        <v/>
       </c>
       <c r="I9" s="7" cm="1">
         <f t="array" ref="I9">_xlfn.IFS(F9="",0,F9="water",11.5, TRUE, 5)</f>
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-      <c r="P9" s="16">
+        <v>15</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Q9" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T9" s="16" t="s">
+      <c r="T9" t="s">
         <v>10</v>
       </c>
-      <c r="U9" s="16" t="str">
+      <c r="U9" t="str">
         <f t="shared" si="4"/>
-        <v>Positive control</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>12</v>
-      </c>
+        <v>test</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="H10" s="7" t="str">
         <f>IF(F10="","", INDEX(Table4[],MATCH(F10,Table4[primer],0),1))</f>
         <v/>
@@ -1714,101 +1687,113 @@
       </c>
       <c r="K10" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="H11" s="7" t="str">
+        <f>IF(F11="","", INDEX(Table4[],MATCH(F11,Table4[primer],0),1))</f>
+        <v/>
+      </c>
+      <c r="I11" s="7" cm="1">
+        <f t="array" ref="I11">_xlfn.IFS(F11="",0,F11="water",11.5, TRUE, 5)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="16">
+      <c r="H12" s="7" t="str">
+        <f>IF(F12="","", INDEX(Table4[],MATCH(F12,Table4[primer],0),1))</f>
+        <v/>
+      </c>
+      <c r="I12" s="7" cm="1">
+        <f t="array" ref="I12">_xlfn.IFS(F12="",0,F12="water",11.5, TRUE, 5)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R10" s="16">
+      <c r="R12">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="U10" s="16" t="str">
+      <c r="T12" t="s">
+        <v>13</v>
+      </c>
+      <c r="U12" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="H11" s="7" t="str">
-        <f>IF(F11="","", INDEX(Table4[],MATCH(F11,Table4[primer],0),1))</f>
-        <v/>
-      </c>
-      <c r="I11" s="7" cm="1">
-        <f t="array" ref="I11">_xlfn.IFS(F11="",0,F11="water",11.5, TRUE, 5)</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="U11" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="H12" s="7" t="str">
-        <f>IF(F12="","", INDEX(Table4[],MATCH(F12,Table4[primer],0),1))</f>
-        <v/>
-      </c>
-      <c r="I12" s="7" cm="1">
-        <f t="array" ref="I12">_xlfn.IFS(F12="",0,F12="water",11.5, TRUE, 5)</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="U12" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
       <c r="H13" s="7" t="str">
         <f>IF(F13="","", INDEX(Table4[],MATCH(F13,Table4[primer],0),1))</f>
         <v/>
@@ -1822,40 +1807,29 @@
       </c>
       <c r="K13" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="16">
+        <v>15</v>
+      </c>
+      <c r="P13">
         <f>COUNTIFS($C$2:$C$97,C13,$B$2:$B$97,B13)</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q13">
         <f>COUNTIFS($E$2:$E$97, E13, $F$2:$F$97, F13)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="16">
+      <c r="R13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="T13" t="s">
         <v>14</v>
       </c>
-      <c r="U13" s="16" t="str">
+      <c r="U13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="H14" s="7" t="str">
         <f>IF(F14="","", INDEX(Table4[],MATCH(F14,Table4[primer],0),1))</f>
         <v/>
@@ -1871,38 +1845,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R14" s="16">
+      <c r="R14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T14" s="18" t="s">
+      <c r="T14" t="s">
         <v>15</v>
       </c>
-      <c r="U14" s="16" t="str">
+      <c r="U14" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="H15" s="7" t="str">
         <f>IF(F15="","", INDEX(Table4[],MATCH(F15,Table4[primer],0),1))</f>
         <v/>
@@ -1918,38 +1881,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="Q15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R15" s="16">
+      <c r="R15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T15" s="18" t="s">
+      <c r="T15" t="s">
         <v>16</v>
       </c>
-      <c r="U15" s="16" t="str">
+      <c r="U15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="18"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="H16" s="7" t="str">
         <f>IF(F16="","", INDEX(Table4[],MATCH(F16,Table4[primer],0),1))</f>
         <v/>
@@ -1965,38 +1917,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P16" s="16">
+      <c r="P16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R16" s="16">
+      <c r="R16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T16" s="18" t="s">
+      <c r="T16" t="s">
         <v>17</v>
       </c>
-      <c r="U16" s="16" t="str">
+      <c r="U16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
-    </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H17" s="7" t="str">
         <f>IF(F17="","", INDEX(Table4[],MATCH(F17,Table4[primer],0),1))</f>
         <v/>
@@ -2012,349 +1953,387 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P17" s="16">
+      <c r="P17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="16">
+      <c r="Q17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R17" s="16">
+      <c r="R17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T17" s="18" t="s">
+      <c r="T17" t="s">
         <v>18</v>
       </c>
-      <c r="U17" s="16" t="str">
+      <c r="U17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-    </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B18" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>21</v>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>105</v>
       </c>
       <c r="H18" s="7" t="str">
         <f>IF(F18="","", INDEX(Table4[],MATCH(F18,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I18" s="7" cm="1">
         <f t="array" ref="I18">_xlfn.IFS(F18="",0,F18="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="P18" s="16">
+        <v>10</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q18" s="16">
+      <c r="Q18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R18" s="16">
+      <c r="R18">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="T18" s="18" t="s">
+      <c r="T18" t="s">
         <v>19</v>
       </c>
-      <c r="U18" s="16" t="str">
+      <c r="U18" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-    </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>105</v>
+      </c>
       <c r="H19" s="7" t="str">
         <f>IF(F19="","", INDEX(Table4[],MATCH(F19,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I19" s="7" cm="1">
         <f t="array" ref="I19">_xlfn.IFS(F19="",0,F19="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="16">
+        <v>10</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T19" t="s">
         <v>20</v>
       </c>
-      <c r="U19" s="16" t="str">
+      <c r="U19" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>105</v>
+      </c>
       <c r="H20" s="7" t="str">
         <f>IF(F20="","", INDEX(Table4[],MATCH(F20,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I20" s="7" cm="1">
         <f t="array" ref="I20">_xlfn.IFS(F20="",0,F20="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="16">
+        <v>10</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R20" s="16">
+      <c r="R20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T20" t="s">
         <v>21</v>
       </c>
-      <c r="U20" s="16" t="str">
+      <c r="U20" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>105</v>
+      </c>
       <c r="H21" s="7" t="str">
         <f>IF(F21="","", INDEX(Table4[],MATCH(F21,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I21" s="7" cm="1">
         <f t="array" ref="I21">_xlfn.IFS(F21="",0,F21="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>22</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="16">
+        <v>10</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T21" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T21" t="s">
         <v>22</v>
       </c>
-      <c r="U21" s="16" t="str">
+      <c r="U21" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>105</v>
+      </c>
       <c r="H22" s="7" t="str">
         <f>IF(F22="","", INDEX(Table4[],MATCH(F22,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I22" s="7" cm="1">
         <f t="array" ref="I22">_xlfn.IFS(F22="",0,F22="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="16">
+        <v>10</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R22" s="16">
+      <c r="R22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T22" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T22" t="s">
         <v>23</v>
       </c>
-      <c r="U22" s="16" t="str">
+      <c r="U22" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
       <c r="H23" s="7" t="str">
         <f>IF(F23="","", INDEX(Table4[],MATCH(F23,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I23" s="7" cm="1">
         <f t="array" ref="I23">_xlfn.IFS(F23="",0,F23="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="16">
+        <v>10</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R23" s="16">
+      <c r="R23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" t="s">
         <v>24</v>
       </c>
-      <c r="U23" s="16" t="str">
+      <c r="U23" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>105</v>
+      </c>
       <c r="H24" s="7" t="str">
         <f>IF(F24="","", INDEX(Table4[],MATCH(F24,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I24" s="7" cm="1">
         <f t="array" ref="I24">_xlfn.IFS(F24="",0,F24="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>25</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="16">
+        <v>10</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R24" s="16">
+      <c r="R24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T24" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T24" t="s">
         <v>25</v>
       </c>
-      <c r="U24" s="16" t="str">
+      <c r="U24" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>105</v>
+      </c>
       <c r="H25" s="7" t="str">
         <f>IF(F25="","", INDEX(Table4[],MATCH(F25,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I25" s="7" cm="1">
         <f t="array" ref="I25">_xlfn.IFS(F25="",0,F25="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="16">
+        <v>10</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R25" s="16">
+      <c r="R25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T25" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T25" t="s">
         <v>26</v>
       </c>
-      <c r="U25" s="16" t="str">
+      <c r="U25" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B26" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>11</v>
-      </c>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H26" s="7" t="str">
         <f>IF(F26="","", INDEX(Table4[],MATCH(F26,Table4[primer],0),1))</f>
         <v/>
@@ -2368,29 +2347,29 @@
       </c>
       <c r="K26" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="P26" s="16">
+        <v>0</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q26" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q26">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R26" s="16">
+      <c r="R26">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="T26" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="T26" t="s">
         <v>27</v>
       </c>
-      <c r="U26" s="16" t="str">
+      <c r="U26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H27" s="7" t="str">
         <f>IF(F27="","", INDEX(Table4[],MATCH(F27,Table4[primer],0),1))</f>
         <v/>
@@ -2406,27 +2385,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P27" s="16">
+      <c r="P27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="16">
+      <c r="Q27">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R27" s="16">
+      <c r="R27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T27" s="16" t="s">
+      <c r="T27" t="s">
         <v>28</v>
       </c>
-      <c r="U27" s="16" t="str">
+      <c r="U27" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H28" s="7" t="str">
         <f>IF(F28="","", INDEX(Table4[],MATCH(F28,Table4[primer],0),1))</f>
         <v/>
@@ -2442,27 +2421,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P28" s="16">
+      <c r="P28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="16">
+      <c r="Q28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R28" s="16">
+      <c r="R28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T28" s="16" t="s">
+      <c r="T28" t="s">
         <v>29</v>
       </c>
-      <c r="U28" s="16" t="str">
+      <c r="U28" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H29" s="7" t="str">
         <f>IF(F29="","", INDEX(Table4[],MATCH(F29,Table4[primer],0),1))</f>
         <v/>
@@ -2478,27 +2457,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P29" s="16">
+      <c r="P29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="16">
+      <c r="Q29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R29" s="16">
+      <c r="R29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T29" s="16" t="s">
+      <c r="T29" t="s">
         <v>30</v>
       </c>
-      <c r="U29" s="16" t="str">
+      <c r="U29" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H30" s="7" t="str">
         <f>IF(F30="","", INDEX(Table4[],MATCH(F30,Table4[primer],0),1))</f>
         <v/>
@@ -2514,27 +2493,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P30" s="16">
+      <c r="P30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="16">
+      <c r="Q30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T30" s="16" t="s">
+      <c r="T30" t="s">
         <v>31</v>
       </c>
-      <c r="U30" s="16" t="str">
+      <c r="U30" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H31" s="7" t="str">
         <f>IF(F31="","", INDEX(Table4[],MATCH(F31,Table4[primer],0),1))</f>
         <v/>
@@ -2550,27 +2529,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P31" s="16">
+      <c r="P31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="16">
+      <c r="Q31">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R31" s="16">
+      <c r="R31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T31" s="16" t="s">
+      <c r="T31" t="s">
         <v>32</v>
       </c>
-      <c r="U31" s="16" t="str">
+      <c r="U31" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H32" s="7" t="str">
         <f>IF(F32="","", INDEX(Table4[],MATCH(F32,Table4[primer],0),1))</f>
         <v/>
@@ -2586,22 +2565,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P32" s="16">
+      <c r="P32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="16">
+      <c r="Q32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R32" s="16">
+      <c r="R32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T32" s="16" t="s">
+      <c r="T32" t="s">
         <v>33</v>
       </c>
-      <c r="U32" s="16" t="str">
+      <c r="U32" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2622,22 +2601,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P33" s="16">
+      <c r="P33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="16">
+      <c r="Q33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R33" s="16">
+      <c r="R33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T33" s="16" t="s">
+      <c r="T33" t="s">
         <v>34</v>
       </c>
-      <c r="U33" s="16" t="str">
+      <c r="U33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2658,22 +2637,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P34" s="16">
+      <c r="P34">
         <f t="shared" ref="P34:P65" si="5">COUNTIFS($C$2:$C$97,C34,$B$2:$B$97,B34)</f>
         <v>0</v>
       </c>
-      <c r="Q34" s="16">
+      <c r="Q34">
         <f t="shared" ref="Q34:Q66" si="6">COUNTIFS($E$2:$E$97, E34, $F$2:$F$97, F34)</f>
         <v>0</v>
       </c>
-      <c r="R34" s="16">
+      <c r="R34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T34" s="16" t="s">
+      <c r="T34" t="s">
         <v>35</v>
       </c>
-      <c r="U34" s="16" t="str">
+      <c r="U34" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2694,22 +2673,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P35" s="16">
+      <c r="P35">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q35" s="16">
+      <c r="Q35">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R35" s="16">
+      <c r="R35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T35" s="16" t="s">
+      <c r="T35" t="s">
         <v>36</v>
       </c>
-      <c r="U35" s="16" t="str">
+      <c r="U35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2730,22 +2709,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P36" s="16">
+      <c r="P36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q36" s="16">
+      <c r="Q36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R36" s="16">
+      <c r="R36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T36" s="16" t="s">
+      <c r="T36" t="s">
         <v>37</v>
       </c>
-      <c r="U36" s="16" t="str">
+      <c r="U36" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2766,22 +2745,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P37" s="16">
+      <c r="P37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q37" s="16">
+      <c r="Q37">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R37" s="16">
+      <c r="R37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T37" s="16" t="s">
+      <c r="T37" t="s">
         <v>38</v>
       </c>
-      <c r="U37" s="16" t="str">
+      <c r="U37" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2802,22 +2781,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P38" s="16">
+      <c r="P38">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q38" s="16">
+      <c r="Q38">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R38" s="16">
+      <c r="R38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T38" s="16" t="s">
+      <c r="T38" t="s">
         <v>39</v>
       </c>
-      <c r="U38" s="16" t="str">
+      <c r="U38" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2838,22 +2817,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P39" s="16">
+      <c r="P39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q39" s="16">
+      <c r="Q39">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R39" s="16">
+      <c r="R39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T39" s="16" t="s">
+      <c r="T39" t="s">
         <v>40</v>
       </c>
-      <c r="U39" s="16" t="str">
+      <c r="U39" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2874,22 +2853,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P40" s="16">
+      <c r="P40">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q40" s="16">
+      <c r="Q40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R40" s="16">
+      <c r="R40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T40" s="16" t="s">
+      <c r="T40" t="s">
         <v>41</v>
       </c>
-      <c r="U40" s="16" t="str">
+      <c r="U40" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2910,22 +2889,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P41" s="16">
+      <c r="P41">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="16">
+      <c r="Q41">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R41" s="16">
+      <c r="R41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T41" s="16" t="s">
+      <c r="T41" t="s">
         <v>42</v>
       </c>
-      <c r="U41" s="16" t="str">
+      <c r="U41" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2946,22 +2925,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P42" s="16">
+      <c r="P42">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="16">
+      <c r="Q42">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R42" s="16">
+      <c r="R42">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T42" s="16" t="s">
+      <c r="T42" t="s">
         <v>43</v>
       </c>
-      <c r="U42" s="16" t="str">
+      <c r="U42" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2982,22 +2961,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P43" s="16">
+      <c r="P43">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q43" s="16">
+      <c r="Q43">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R43" s="16">
+      <c r="R43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T43" s="16" t="s">
+      <c r="T43" t="s">
         <v>44</v>
       </c>
-      <c r="U43" s="16" t="str">
+      <c r="U43" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3018,22 +2997,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P44" s="16">
+      <c r="P44">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q44" s="16">
+      <c r="Q44">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R44" s="16">
+      <c r="R44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T44" s="16" t="s">
+      <c r="T44" t="s">
         <v>45</v>
       </c>
-      <c r="U44" s="16" t="str">
+      <c r="U44" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3054,22 +3033,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P45" s="16">
+      <c r="P45">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q45" s="16">
+      <c r="Q45">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R45" s="16">
+      <c r="R45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T45" s="16" t="s">
+      <c r="T45" t="s">
         <v>46</v>
       </c>
-      <c r="U45" s="16" t="str">
+      <c r="U45" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3090,22 +3069,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P46" s="16">
+      <c r="P46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q46" s="16">
+      <c r="Q46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R46" s="16">
+      <c r="R46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T46" s="16" t="s">
+      <c r="T46" t="s">
         <v>47</v>
       </c>
-      <c r="U46" s="16" t="str">
+      <c r="U46" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3126,22 +3105,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P47" s="16">
+      <c r="P47">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q47" s="16">
+      <c r="Q47">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R47" s="16">
+      <c r="R47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T47" s="16" t="s">
+      <c r="T47" t="s">
         <v>48</v>
       </c>
-      <c r="U47" s="16" t="str">
+      <c r="U47" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3162,22 +3141,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P48" s="16">
+      <c r="P48">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q48" s="16">
+      <c r="Q48">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R48" s="16">
+      <c r="R48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T48" s="16" t="s">
+      <c r="T48" t="s">
         <v>49</v>
       </c>
-      <c r="U48" s="16" t="str">
+      <c r="U48" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3198,22 +3177,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P49" s="16">
+      <c r="P49">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q49" s="16">
+      <c r="Q49">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R49" s="16">
+      <c r="R49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T49" s="16" t="s">
+      <c r="T49" t="s">
         <v>50</v>
       </c>
-      <c r="U49" s="16" t="str">
+      <c r="U49" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3234,22 +3213,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P50" s="16">
+      <c r="P50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q50" s="16">
+      <c r="Q50">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R50" s="16">
+      <c r="R50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T50" s="16" t="s">
+      <c r="T50" t="s">
         <v>51</v>
       </c>
-      <c r="U50" s="16" t="str">
+      <c r="U50" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3270,22 +3249,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P51" s="16">
+      <c r="P51">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q51" s="16">
+      <c r="Q51">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R51" s="16">
+      <c r="R51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T51" s="16" t="s">
+      <c r="T51" t="s">
         <v>52</v>
       </c>
-      <c r="U51" s="16" t="str">
+      <c r="U51" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3306,22 +3285,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P52" s="16">
+      <c r="P52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q52" s="16">
+      <c r="Q52">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R52" s="16">
+      <c r="R52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T52" s="16" t="s">
+      <c r="T52" t="s">
         <v>53</v>
       </c>
-      <c r="U52" s="16" t="str">
+      <c r="U52" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3342,22 +3321,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P53" s="16">
+      <c r="P53">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q53" s="16">
+      <c r="Q53">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R53" s="16">
+      <c r="R53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T53" s="16" t="s">
+      <c r="T53" t="s">
         <v>54</v>
       </c>
-      <c r="U53" s="16" t="str">
+      <c r="U53" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3378,22 +3357,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P54" s="16">
+      <c r="P54">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q54" s="16">
+      <c r="Q54">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R54" s="16">
+      <c r="R54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T54" s="16" t="s">
+      <c r="T54" t="s">
         <v>55</v>
       </c>
-      <c r="U54" s="16" t="str">
+      <c r="U54" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3414,22 +3393,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P55" s="16">
+      <c r="P55">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q55" s="16">
+      <c r="Q55">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R55" s="16">
+      <c r="R55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T55" s="16" t="s">
+      <c r="T55" t="s">
         <v>56</v>
       </c>
-      <c r="U55" s="16" t="str">
+      <c r="U55" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3450,22 +3429,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P56" s="16">
+      <c r="P56">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q56" s="16">
+      <c r="Q56">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R56" s="16">
+      <c r="R56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T56" s="16" t="s">
+      <c r="T56" t="s">
         <v>57</v>
       </c>
-      <c r="U56" s="16" t="str">
+      <c r="U56" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3486,22 +3465,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P57" s="16">
+      <c r="P57">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q57" s="16">
+      <c r="Q57">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R57" s="16">
+      <c r="R57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T57" s="16" t="s">
+      <c r="T57" t="s">
         <v>58</v>
       </c>
-      <c r="U57" s="16" t="str">
+      <c r="U57" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3522,22 +3501,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P58" s="16">
+      <c r="P58">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q58" s="16">
+      <c r="Q58">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R58" s="16">
+      <c r="R58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T58" s="16" t="s">
+      <c r="T58" t="s">
         <v>59</v>
       </c>
-      <c r="U58" s="16" t="str">
+      <c r="U58" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3558,22 +3537,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P59" s="16">
+      <c r="P59">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q59" s="16">
+      <c r="Q59">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R59" s="16">
+      <c r="R59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T59" s="16" t="s">
+      <c r="T59" t="s">
         <v>60</v>
       </c>
-      <c r="U59" s="16" t="str">
+      <c r="U59" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3594,22 +3573,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P60" s="16">
+      <c r="P60">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q60" s="16">
+      <c r="Q60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R60" s="16">
+      <c r="R60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T60" s="16" t="s">
+      <c r="T60" t="s">
         <v>61</v>
       </c>
-      <c r="U60" s="16" t="str">
+      <c r="U60" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3630,22 +3609,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P61" s="16">
+      <c r="P61">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q61" s="16">
+      <c r="Q61">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R61" s="16">
+      <c r="R61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T61" s="16" t="s">
+      <c r="T61" t="s">
         <v>62</v>
       </c>
-      <c r="U61" s="16" t="str">
+      <c r="U61" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3666,22 +3645,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P62" s="16">
+      <c r="P62">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q62" s="16">
+      <c r="Q62">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R62" s="16">
+      <c r="R62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T62" s="16" t="s">
+      <c r="T62" t="s">
         <v>63</v>
       </c>
-      <c r="U62" s="16" t="str">
+      <c r="U62" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3702,22 +3681,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P63" s="16">
+      <c r="P63">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q63" s="16">
+      <c r="Q63">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R63" s="16">
+      <c r="R63">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T63" s="16" t="s">
+      <c r="T63" t="s">
         <v>64</v>
       </c>
-      <c r="U63" s="16" t="str">
+      <c r="U63" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3738,22 +3717,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P64" s="16">
+      <c r="P64">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q64" s="16">
+      <c r="Q64">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R64" s="16">
+      <c r="R64">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T64" s="16" t="s">
+      <c r="T64" t="s">
         <v>65</v>
       </c>
-      <c r="U64" s="16" t="str">
+      <c r="U64" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3774,22 +3753,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P65" s="16">
+      <c r="P65">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q65" s="16">
+      <c r="Q65">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R65" s="16">
+      <c r="R65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T65" s="16" t="s">
+      <c r="T65" t="s">
         <v>66</v>
       </c>
-      <c r="U65" s="16" t="str">
+      <c r="U65" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3810,22 +3789,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P66" s="16">
+      <c r="P66">
         <f t="shared" ref="P66:P97" si="7">COUNTIFS($C$2:$C$97,C66,$B$2:$B$97,B66)</f>
         <v>0</v>
       </c>
-      <c r="Q66" s="16">
+      <c r="Q66">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R66" s="16">
+      <c r="R66">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T66" s="16" t="s">
+      <c r="T66" t="s">
         <v>67</v>
       </c>
-      <c r="U66" s="16" t="str">
+      <c r="U66" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3846,22 +3825,22 @@
         <f t="shared" ref="K67:K97" si="8">IF(OR(C67 = "",B67=""),0,15-I67)</f>
         <v>0</v>
       </c>
-      <c r="P67" s="16">
+      <c r="P67">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q67" s="16">
+      <c r="Q67">
         <f t="shared" ref="Q67:Q97" si="9">COUNTIFS($E$2:$E$97, E67, $F$2:$F$97, F67)</f>
         <v>0</v>
       </c>
-      <c r="R67" s="16">
+      <c r="R67">
         <f t="shared" ref="R67:R97" si="10">I67+K67</f>
         <v>0</v>
       </c>
-      <c r="T67" s="16" t="s">
+      <c r="T67" t="s">
         <v>68</v>
       </c>
-      <c r="U67" s="16" t="str">
+      <c r="U67" t="str">
         <f t="shared" ref="U67:U97" si="11">TEXT(D67,"")</f>
         <v/>
       </c>
@@ -3882,22 +3861,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P68" s="16">
+      <c r="P68">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q68" s="16">
+      <c r="Q68">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R68" s="16">
+      <c r="R68">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T68" s="16" t="s">
+      <c r="T68" t="s">
         <v>69</v>
       </c>
-      <c r="U68" s="16" t="str">
+      <c r="U68" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -3918,22 +3897,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P69" s="16">
+      <c r="P69">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q69" s="16">
+      <c r="Q69">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R69" s="16">
+      <c r="R69">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T69" s="16" t="s">
+      <c r="T69" t="s">
         <v>70</v>
       </c>
-      <c r="U69" s="16" t="str">
+      <c r="U69" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -3954,22 +3933,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P70" s="16">
+      <c r="P70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q70" s="16">
+      <c r="Q70">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R70" s="16">
+      <c r="R70">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T70" s="16" t="s">
+      <c r="T70" t="s">
         <v>71</v>
       </c>
-      <c r="U70" s="16" t="str">
+      <c r="U70" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -3990,22 +3969,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P71" s="16">
+      <c r="P71">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q71" s="16">
+      <c r="Q71">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R71" s="16">
+      <c r="R71">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T71" s="16" t="s">
+      <c r="T71" t="s">
         <v>72</v>
       </c>
-      <c r="U71" s="16" t="str">
+      <c r="U71" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4026,22 +4005,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P72" s="16">
+      <c r="P72">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q72" s="16">
+      <c r="Q72">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R72" s="16">
+      <c r="R72">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T72" s="16" t="s">
+      <c r="T72" t="s">
         <v>73</v>
       </c>
-      <c r="U72" s="16" t="str">
+      <c r="U72" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4062,22 +4041,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P73" s="16">
+      <c r="P73">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q73" s="16">
+      <c r="Q73">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R73" s="16">
+      <c r="R73">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T73" s="16" t="s">
+      <c r="T73" t="s">
         <v>74</v>
       </c>
-      <c r="U73" s="16" t="str">
+      <c r="U73" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4098,22 +4077,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P74" s="16">
+      <c r="P74">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q74" s="16">
+      <c r="Q74">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R74" s="16">
+      <c r="R74">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T74" s="16" t="s">
+      <c r="T74" t="s">
         <v>75</v>
       </c>
-      <c r="U74" s="16" t="str">
+      <c r="U74" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4134,22 +4113,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P75" s="16">
+      <c r="P75">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q75" s="16">
+      <c r="Q75">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R75" s="16">
+      <c r="R75">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T75" s="16" t="s">
+      <c r="T75" t="s">
         <v>76</v>
       </c>
-      <c r="U75" s="16" t="str">
+      <c r="U75" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4170,22 +4149,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P76" s="16">
+      <c r="P76">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q76" s="16">
+      <c r="Q76">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R76" s="16">
+      <c r="R76">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T76" s="16" t="s">
+      <c r="T76" t="s">
         <v>77</v>
       </c>
-      <c r="U76" s="16" t="str">
+      <c r="U76" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4206,22 +4185,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P77" s="16">
+      <c r="P77">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q77" s="16">
+      <c r="Q77">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R77" s="16">
+      <c r="R77">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T77" s="16" t="s">
+      <c r="T77" t="s">
         <v>78</v>
       </c>
-      <c r="U77" s="16" t="str">
+      <c r="U77" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4242,22 +4221,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P78" s="16">
+      <c r="P78">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q78" s="16">
+      <c r="Q78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R78" s="16">
+      <c r="R78">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T78" s="16" t="s">
+      <c r="T78" t="s">
         <v>79</v>
       </c>
-      <c r="U78" s="16" t="str">
+      <c r="U78" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4278,22 +4257,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P79" s="16">
+      <c r="P79">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q79" s="16">
+      <c r="Q79">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R79" s="16">
+      <c r="R79">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T79" s="16" t="s">
+      <c r="T79" t="s">
         <v>80</v>
       </c>
-      <c r="U79" s="16" t="str">
+      <c r="U79" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4314,22 +4293,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P80" s="16">
+      <c r="P80">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q80" s="16">
+      <c r="Q80">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R80" s="16">
+      <c r="R80">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T80" s="16" t="s">
+      <c r="T80" t="s">
         <v>81</v>
       </c>
-      <c r="U80" s="16" t="str">
+      <c r="U80" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4350,22 +4329,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P81" s="16">
+      <c r="P81">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q81" s="16">
+      <c r="Q81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R81" s="16">
+      <c r="R81">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T81" s="16" t="s">
+      <c r="T81" t="s">
         <v>82</v>
       </c>
-      <c r="U81" s="16" t="str">
+      <c r="U81" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4386,22 +4365,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P82" s="16">
+      <c r="P82">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q82" s="16">
+      <c r="Q82">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R82" s="16">
+      <c r="R82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T82" s="16" t="s">
+      <c r="T82" t="s">
         <v>83</v>
       </c>
-      <c r="U82" s="16" t="str">
+      <c r="U82" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4422,22 +4401,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P83" s="16">
+      <c r="P83">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q83" s="16">
+      <c r="Q83">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R83" s="16">
+      <c r="R83">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T83" s="16" t="s">
+      <c r="T83" t="s">
         <v>84</v>
       </c>
-      <c r="U83" s="16" t="str">
+      <c r="U83" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4458,22 +4437,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P84" s="16">
+      <c r="P84">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q84" s="16">
+      <c r="Q84">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R84" s="16">
+      <c r="R84">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T84" s="16" t="s">
+      <c r="T84" t="s">
         <v>85</v>
       </c>
-      <c r="U84" s="16" t="str">
+      <c r="U84" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4494,22 +4473,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P85" s="16">
+      <c r="P85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q85" s="16">
+      <c r="Q85">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R85" s="16">
+      <c r="R85">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T85" s="16" t="s">
+      <c r="T85" t="s">
         <v>86</v>
       </c>
-      <c r="U85" s="16" t="str">
+      <c r="U85" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4530,22 +4509,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P86" s="16">
+      <c r="P86">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q86" s="16">
+      <c r="Q86">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R86" s="16">
+      <c r="R86">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T86" s="16" t="s">
+      <c r="T86" t="s">
         <v>87</v>
       </c>
-      <c r="U86" s="16" t="str">
+      <c r="U86" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4566,22 +4545,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P87" s="16">
+      <c r="P87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q87" s="16">
+      <c r="Q87">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R87" s="16">
+      <c r="R87">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T87" s="16" t="s">
+      <c r="T87" t="s">
         <v>88</v>
       </c>
-      <c r="U87" s="16" t="str">
+      <c r="U87" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4602,22 +4581,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P88" s="16">
+      <c r="P88">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q88" s="16">
+      <c r="Q88">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R88" s="16">
+      <c r="R88">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T88" s="16" t="s">
+      <c r="T88" t="s">
         <v>89</v>
       </c>
-      <c r="U88" s="16" t="str">
+      <c r="U88" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4638,22 +4617,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P89" s="16">
+      <c r="P89">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q89" s="16">
+      <c r="Q89">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R89" s="16">
+      <c r="R89">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T89" s="16" t="s">
+      <c r="T89" t="s">
         <v>90</v>
       </c>
-      <c r="U89" s="16" t="str">
+      <c r="U89" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4674,22 +4653,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P90" s="16">
+      <c r="P90">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q90" s="16">
+      <c r="Q90">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R90" s="16">
+      <c r="R90">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T90" s="16" t="s">
+      <c r="T90" t="s">
         <v>91</v>
       </c>
-      <c r="U90" s="16" t="str">
+      <c r="U90" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4710,22 +4689,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P91" s="16">
+      <c r="P91">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q91" s="16">
+      <c r="Q91">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R91" s="16">
+      <c r="R91">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T91" s="16" t="s">
+      <c r="T91" t="s">
         <v>92</v>
       </c>
-      <c r="U91" s="16" t="str">
+      <c r="U91" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4746,22 +4725,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P92" s="16">
+      <c r="P92">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q92" s="16">
+      <c r="Q92">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R92" s="16">
+      <c r="R92">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T92" s="16" t="s">
+      <c r="T92" t="s">
         <v>93</v>
       </c>
-      <c r="U92" s="16" t="str">
+      <c r="U92" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4782,22 +4761,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P93" s="16">
+      <c r="P93">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q93" s="16">
+      <c r="Q93">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R93" s="16">
+      <c r="R93">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T93" s="16" t="s">
+      <c r="T93" t="s">
         <v>94</v>
       </c>
-      <c r="U93" s="16" t="str">
+      <c r="U93" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4818,22 +4797,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P94" s="16">
+      <c r="P94">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q94" s="16">
+      <c r="Q94">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R94" s="16">
+      <c r="R94">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T94" s="16" t="s">
+      <c r="T94" t="s">
         <v>95</v>
       </c>
-      <c r="U94" s="16" t="str">
+      <c r="U94" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4854,22 +4833,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P95" s="16">
+      <c r="P95">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q95" s="16">
+      <c r="Q95">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R95" s="16">
+      <c r="R95">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T95" s="16" t="s">
+      <c r="T95" t="s">
         <v>96</v>
       </c>
-      <c r="U95" s="16" t="str">
+      <c r="U95" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4890,22 +4869,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P96" s="16">
+      <c r="P96">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q96" s="16">
+      <c r="Q96">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R96" s="16">
+      <c r="R96">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T96" s="16" t="s">
+      <c r="T96" t="s">
         <v>97</v>
       </c>
-      <c r="U96" s="16" t="str">
+      <c r="U96" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4926,22 +4905,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P97" s="16">
+      <c r="P97">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q97" s="16">
+      <c r="Q97">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R97" s="16">
+      <c r="R97">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T97" s="16" t="s">
+      <c r="T97" t="s">
         <v>98</v>
       </c>
-      <c r="U97" s="16" t="str">
+      <c r="U97" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5007,7 +4986,7 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5359,10 +5338,10 @@
         <v>46</v>
       </c>
       <c r="B25" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" t="s">
         <v>188</v>
-      </c>
-      <c r="C25" t="s">
-        <v>189</v>
       </c>
       <c r="F25" t="s">
         <v>145</v>
@@ -5461,7 +5440,7 @@
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J37" t="s">
         <v>38</v>
@@ -5811,20 +5790,20 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>IF(master!B2="plate",master!C2, "")</f>
-        <v>A01</v>
+        <v>A02</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
         <f>IF(master!B2="plate",master!K2,0)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>IF(master!B3="plate",master!C3, "")</f>
-        <v>B01</v>
+        <v>B02</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -5837,20 +5816,20 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>IF(master!B4="plate",master!C4, "")</f>
-        <v>C01</v>
+        <v>C02</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1">
         <f>IF(master!B4="plate",master!K4,0)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>IF(master!B5="plate",master!C5, "")</f>
-        <v>D01</v>
+        <v>D02</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -5863,7 +5842,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>IF(master!B6="plate",master!C6, "")</f>
-        <v>E01</v>
+        <v>E02</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -5876,53 +5855,53 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>IF(master!B7="plate",master!C7, "")</f>
-        <v/>
+        <v>F02</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1">
         <f>IF(master!B7="plate",master!K7,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f>IF(master!B8="plate",master!C8, "")</f>
-        <v/>
+        <v>G02</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>IF(master!B8="plate",master!K8,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>IF(master!B9="plate",master!C9, "")</f>
-        <v/>
+        <v>H02</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1">
         <f>IF(master!B9="plate",master!K9,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>IF(master!B10="plate",master!C10, "")</f>
-        <v>B02</v>
+        <v/>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1">
         <f>IF(master!B10="plate",master!K10,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -6019,14 +5998,14 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(master!B18="plate",master!C18, "")</f>
-        <v>C03</v>
+        <v/>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1">
         <f>IF(master!B18="plate",master!K18,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -7163,40 +7142,40 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>IF(master!B7="strip",master!C7,"")</f>
-        <v>F01</v>
+        <v/>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1">
         <f>IF(master!B7="strip",master!K7,0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f>IF(master!B8="strip",master!C8,"")</f>
-        <v>H12</v>
+        <v/>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>IF(master!B8="strip",master!K8,0)</f>
-        <v>3.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>IF(master!B9="strip",master!C9,"")</f>
-        <v>H12</v>
+        <v/>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1">
         <f>IF(master!B9="strip",master!K9,0)</f>
-        <v>3.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -7228,27 +7207,27 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>IF(master!B12="strip",master!C12,"")</f>
-        <v/>
+        <v>E02</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <f>IF(master!B12="strip",master!K12,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f>IF(master!B13="strip",master!C13,"")</f>
-        <v/>
+        <v>B05</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="1">
         <f>IF(master!B13="strip",master!K13,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -7306,118 +7285,118 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(master!B18="strip",master!C18,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1">
         <f>IF(master!B18="strip",master!K18,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f>IF(master!B19="strip",master!C19,"")</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1">
         <f>IF(master!B19="strip",master!K19,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f>IF(master!B20="strip",master!C20,"")</f>
-        <v/>
+        <v>C01</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="1">
         <f>IF(master!B20="strip",master!K20,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f>IF(master!B21="strip",master!C21,"")</f>
-        <v/>
+        <v>D01</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="1">
         <f>IF(master!B21="strip",master!K21,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
         <f>IF(master!B22="strip",master!C22,"")</f>
-        <v/>
+        <v>E01</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1">
         <f>IF(master!B22="strip",master!K22,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f>IF(master!B23="strip",master!C23,"")</f>
-        <v/>
+        <v>F01</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="1">
         <f>IF(master!B23="strip",master!K23,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <f>IF(master!B24="strip",master!C24,"")</f>
-        <v/>
+        <v>G01</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="1">
         <f>IF(master!B24="strip",master!K24,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <f>IF(master!B25="strip",master!C25,"")</f>
-        <v/>
+        <v>H01</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="1">
         <f>IF(master!B25="strip",master!K25,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
         <f>IF(master!B26="strip",master!C26,"")</f>
-        <v>A02</v>
+        <v/>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="1">
         <f>IF(master!B26="strip",master!K26,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -8387,14 +8366,14 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>IF(ISTEXT(master!F2),master!H2,"")</f>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
         <f>master!I2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -8413,14 +8392,14 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>IF(ISTEXT(master!F4),master!H4,"")</f>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1">
         <f>master!I4</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -8452,40 +8431,40 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>IF(ISTEXT(master!F7),master!H7,"")</f>
-        <v>C02</v>
+        <v/>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1">
         <f>master!I7</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f>IF(ISTEXT(master!F8),master!H8,"")</f>
-        <v>D05</v>
+        <v/>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>master!I8</f>
-        <v>11.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>IF(ISTEXT(master!F9),master!H9,"")</f>
-        <v>D05</v>
+        <v/>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1">
         <f>master!I9</f>
-        <v>11.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -8595,105 +8574,105 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(ISTEXT(master!F18),master!H18,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1">
         <f>master!I18</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f>IF(ISTEXT(master!F19),master!H19,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1">
         <f>master!I19</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f>IF(ISTEXT(master!F20),master!H20,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="1">
         <f>master!I20</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f>IF(ISTEXT(master!F21),master!H21,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="1">
         <f>master!I21</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
         <f>IF(ISTEXT(master!F22),master!H22,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1">
         <f>master!I22</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f>IF(ISTEXT(master!F23),master!H23,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="1">
         <f>master!I23</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <f>IF(ISTEXT(master!F24),master!H24,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="1">
         <f>master!I24</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <f>IF(ISTEXT(master!F25),master!H25,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="1">
         <f>master!I25</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -9650,7 +9629,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9662,37 +9641,37 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>176</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>177</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>178</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>180</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>181</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>182</v>
-      </c>
-      <c r="I1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>source_plate!A2</f>
-        <v>A01</v>
+        <v>A02</v>
       </c>
       <c r="B2" t="str">
         <f>source_plate!B2</f>
@@ -9700,7 +9679,7 @@
       </c>
       <c r="C2">
         <f>source_plate!C2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2" t="str">
         <f>source_strip!A2</f>
@@ -9716,7 +9695,7 @@
       </c>
       <c r="G2" t="str">
         <f>source_tube!A2</f>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="H2" t="str">
         <f>source_tube!B2</f>
@@ -9724,13 +9703,13 @@
       </c>
       <c r="I2">
         <f>source_tube!C2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>source_plate!A3</f>
-        <v>B01</v>
+        <v>B02</v>
       </c>
       <c r="B3" t="str">
         <f>source_plate!B3</f>
@@ -9768,7 +9747,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>source_plate!A4</f>
-        <v>C01</v>
+        <v>C02</v>
       </c>
       <c r="B4" t="str">
         <f>source_plate!B4</f>
@@ -9776,7 +9755,7 @@
       </c>
       <c r="C4">
         <f>source_plate!C4</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" t="str">
         <f>source_strip!A4</f>
@@ -9792,7 +9771,7 @@
       </c>
       <c r="G4" t="str">
         <f>source_tube!A4</f>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="H4" t="str">
         <f>source_tube!B4</f>
@@ -9800,13 +9779,13 @@
       </c>
       <c r="I4">
         <f>source_tube!C4</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>source_plate!A5</f>
-        <v>D01</v>
+        <v>D02</v>
       </c>
       <c r="B5" t="str">
         <f>source_plate!B5</f>
@@ -9844,7 +9823,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>source_plate!A6</f>
-        <v>E01</v>
+        <v>E02</v>
       </c>
       <c r="B6" t="str">
         <f>source_plate!B6</f>
@@ -9882,7 +9861,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>source_plate!A7</f>
-        <v/>
+        <v>F02</v>
       </c>
       <c r="B7" t="str">
         <f>source_plate!B7</f>
@@ -9890,11 +9869,11 @@
       </c>
       <c r="C7">
         <f>source_plate!C7</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D7" t="str">
         <f>source_strip!A7</f>
-        <v>F01</v>
+        <v/>
       </c>
       <c r="E7" t="str">
         <f>source_strip!B7</f>
@@ -9902,11 +9881,11 @@
       </c>
       <c r="F7">
         <f>source_strip!C7</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G7" t="str">
         <f>source_tube!A7</f>
-        <v>C02</v>
+        <v/>
       </c>
       <c r="H7" t="str">
         <f>source_tube!B7</f>
@@ -9914,13 +9893,13 @@
       </c>
       <c r="I7">
         <f>source_tube!C7</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>source_plate!A8</f>
-        <v/>
+        <v>G02</v>
       </c>
       <c r="B8" t="str">
         <f>source_plate!B8</f>
@@ -9928,11 +9907,11 @@
       </c>
       <c r="C8">
         <f>source_plate!C8</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D8" t="str">
         <f>source_strip!A8</f>
-        <v>H12</v>
+        <v/>
       </c>
       <c r="E8" t="str">
         <f>source_strip!B8</f>
@@ -9940,11 +9919,11 @@
       </c>
       <c r="F8">
         <f>source_strip!C8</f>
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="G8" t="str">
         <f>source_tube!A8</f>
-        <v>D05</v>
+        <v/>
       </c>
       <c r="H8" t="str">
         <f>source_tube!B8</f>
@@ -9952,13 +9931,13 @@
       </c>
       <c r="I8">
         <f>source_tube!C8</f>
-        <v>11.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>source_plate!A9</f>
-        <v/>
+        <v>H02</v>
       </c>
       <c r="B9" t="str">
         <f>source_plate!B9</f>
@@ -9966,11 +9945,11 @@
       </c>
       <c r="C9">
         <f>source_plate!C9</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D9" t="str">
         <f>source_strip!A9</f>
-        <v>H12</v>
+        <v/>
       </c>
       <c r="E9" t="str">
         <f>source_strip!B9</f>
@@ -9978,11 +9957,11 @@
       </c>
       <c r="F9">
         <f>source_strip!C9</f>
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="G9" t="str">
         <f>source_tube!A9</f>
-        <v>D05</v>
+        <v/>
       </c>
       <c r="H9" t="str">
         <f>source_tube!B9</f>
@@ -9990,13 +9969,13 @@
       </c>
       <c r="I9">
         <f>source_tube!C9</f>
-        <v>11.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>source_plate!A10</f>
-        <v>B02</v>
+        <v/>
       </c>
       <c r="B10" t="str">
         <f>source_plate!B10</f>
@@ -10004,7 +9983,7 @@
       </c>
       <c r="C10">
         <f>source_plate!C10</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D10" t="str">
         <f>source_strip!A10</f>
@@ -10084,7 +10063,7 @@
       </c>
       <c r="D12" t="str">
         <f>source_strip!A12</f>
-        <v/>
+        <v>E02</v>
       </c>
       <c r="E12" t="str">
         <f>source_strip!B12</f>
@@ -10092,7 +10071,7 @@
       </c>
       <c r="F12">
         <f>source_strip!C12</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G12" t="str">
         <f>source_tube!A12</f>
@@ -10122,7 +10101,7 @@
       </c>
       <c r="D13" t="str">
         <f>source_strip!A13</f>
-        <v/>
+        <v>B05</v>
       </c>
       <c r="E13" t="str">
         <f>source_strip!B13</f>
@@ -10130,7 +10109,7 @@
       </c>
       <c r="F13">
         <f>source_strip!C13</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G13" t="str">
         <f>source_tube!A13</f>
@@ -10300,7 +10279,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>source_plate!A18</f>
-        <v>C03</v>
+        <v/>
       </c>
       <c r="B18" t="str">
         <f>source_plate!B18</f>
@@ -10308,11 +10287,11 @@
       </c>
       <c r="C18">
         <f>source_plate!C18</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>source_strip!A18</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="E18" t="str">
         <f>source_strip!B18</f>
@@ -10320,11 +10299,11 @@
       </c>
       <c r="F18">
         <f>source_strip!C18</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G18" t="str">
         <f>source_tube!A18</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H18" t="str">
         <f>source_tube!B18</f>
@@ -10332,7 +10311,7 @@
       </c>
       <c r="I18">
         <f>source_tube!C18</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -10350,7 +10329,7 @@
       </c>
       <c r="D19" t="str">
         <f>source_strip!A19</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="E19" t="str">
         <f>source_strip!B19</f>
@@ -10358,11 +10337,11 @@
       </c>
       <c r="F19">
         <f>source_strip!C19</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G19" t="str">
         <f>source_tube!A19</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H19" t="str">
         <f>source_tube!B19</f>
@@ -10370,7 +10349,7 @@
       </c>
       <c r="I19">
         <f>source_tube!C19</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -10388,7 +10367,7 @@
       </c>
       <c r="D20" t="str">
         <f>source_strip!A20</f>
-        <v/>
+        <v>C01</v>
       </c>
       <c r="E20" t="str">
         <f>source_strip!B20</f>
@@ -10396,11 +10375,11 @@
       </c>
       <c r="F20">
         <f>source_strip!C20</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G20" t="str">
         <f>source_tube!A20</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H20" t="str">
         <f>source_tube!B20</f>
@@ -10408,7 +10387,7 @@
       </c>
       <c r="I20">
         <f>source_tube!C20</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -10426,7 +10405,7 @@
       </c>
       <c r="D21" t="str">
         <f>source_strip!A21</f>
-        <v/>
+        <v>D01</v>
       </c>
       <c r="E21" t="str">
         <f>source_strip!B21</f>
@@ -10434,11 +10413,11 @@
       </c>
       <c r="F21">
         <f>source_strip!C21</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G21" t="str">
         <f>source_tube!A21</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H21" t="str">
         <f>source_tube!B21</f>
@@ -10446,7 +10425,7 @@
       </c>
       <c r="I21">
         <f>source_tube!C21</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -10464,7 +10443,7 @@
       </c>
       <c r="D22" t="str">
         <f>source_strip!A22</f>
-        <v/>
+        <v>E01</v>
       </c>
       <c r="E22" t="str">
         <f>source_strip!B22</f>
@@ -10472,11 +10451,11 @@
       </c>
       <c r="F22">
         <f>source_strip!C22</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G22" t="str">
         <f>source_tube!A22</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H22" t="str">
         <f>source_tube!B22</f>
@@ -10484,7 +10463,7 @@
       </c>
       <c r="I22">
         <f>source_tube!C22</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -10502,7 +10481,7 @@
       </c>
       <c r="D23" t="str">
         <f>source_strip!A23</f>
-        <v/>
+        <v>F01</v>
       </c>
       <c r="E23" t="str">
         <f>source_strip!B23</f>
@@ -10510,11 +10489,11 @@
       </c>
       <c r="F23">
         <f>source_strip!C23</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G23" t="str">
         <f>source_tube!A23</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H23" t="str">
         <f>source_tube!B23</f>
@@ -10522,7 +10501,7 @@
       </c>
       <c r="I23">
         <f>source_tube!C23</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -10540,7 +10519,7 @@
       </c>
       <c r="D24" t="str">
         <f>source_strip!A24</f>
-        <v/>
+        <v>G01</v>
       </c>
       <c r="E24" t="str">
         <f>source_strip!B24</f>
@@ -10548,11 +10527,11 @@
       </c>
       <c r="F24">
         <f>source_strip!C24</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G24" t="str">
         <f>source_tube!A24</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H24" t="str">
         <f>source_tube!B24</f>
@@ -10560,7 +10539,7 @@
       </c>
       <c r="I24">
         <f>source_tube!C24</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -10578,7 +10557,7 @@
       </c>
       <c r="D25" t="str">
         <f>source_strip!A25</f>
-        <v/>
+        <v>H01</v>
       </c>
       <c r="E25" t="str">
         <f>source_strip!B25</f>
@@ -10586,11 +10565,11 @@
       </c>
       <c r="F25">
         <f>source_strip!C25</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G25" t="str">
         <f>source_tube!A25</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H25" t="str">
         <f>source_tube!B25</f>
@@ -10598,7 +10577,7 @@
       </c>
       <c r="I25">
         <f>source_tube!C25</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -10616,7 +10595,7 @@
       </c>
       <c r="D26" t="str">
         <f>source_strip!A26</f>
-        <v>A02</v>
+        <v/>
       </c>
       <c r="E26" t="str">
         <f>source_strip!B26</f>
@@ -10624,7 +10603,7 @@
       </c>
       <c r="F26">
         <f>source_strip!C26</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G26" t="str">
         <f>source_tube!A26</f>
@@ -13344,21 +13323,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FDAF843F15E65A4EA1FFB0CF193B74E3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd4433bf6f24a726161ac457e21002bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1a61fc9-c776-4dd1-85b5-f7d58768ba79" xmlns:ns4="3f421247-72bc-4b61-a591-0b56f96ae993" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d66d7a13b7b51360e8b1c095fb39c19" ns3:_="" ns4:_="">
     <xsd:import namespace="e1a61fc9-c776-4dd1-85b5-f7d58768ba79"/>
@@ -13587,15 +13557,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79D86924-57C1-45D5-9E44-D526494DB02F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CD12B7-1FA3-4B61-BDAE-DF4259CEDD3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -13612,7 +13583,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E774FF9-2144-4DC7-8F36-E7E064C7C739}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13629,4 +13600,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79D86924-57C1-45D5-9E44-D526494DB02F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
full column transfer working with volumes
</commit_message>
<xml_diff>
--- a/templates/01-sanger-master-v3.xlsx
+++ b/templates/01-sanger-master-v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelangelov/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB42C825-8B0A-834E-92E8-76FE7935A5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA03F48A-ACA0-6B41-ABA3-02B387C7E279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="190">
   <si>
     <t>source_well</t>
   </si>
@@ -554,12 +554,6 @@
   </si>
   <si>
     <t>bcl_primer</t>
-  </si>
-  <si>
-    <t>3F</t>
-  </si>
-  <si>
-    <t>3R</t>
   </si>
   <si>
     <t>bcl_primer_pos</t>
@@ -1205,7 +1199,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1249,36 +1243,36 @@
       </c>
       <c r="G1" s="11"/>
       <c r="H1" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
       <c r="P1" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="S1" s="12"/>
       <c r="T1" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -1339,9 +1333,6 @@
       <c r="D3" t="s">
         <v>162</v>
       </c>
-      <c r="E3" t="s">
-        <v>165</v>
-      </c>
       <c r="H3" s="7" t="str">
         <f>IF(F3="","", INDEX(Table4[],MATCH(F3,Table4[primer],0),1))</f>
         <v/>
@@ -1406,7 +1397,7 @@
         <v>15</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
@@ -1438,9 +1429,6 @@
       <c r="D5" t="s">
         <v>162</v>
       </c>
-      <c r="E5" t="s">
-        <v>164</v>
-      </c>
       <c r="H5" s="7" t="str">
         <f>IF(F5="","", INDEX(Table4[],MATCH(F5,Table4[primer],0),1))</f>
         <v/>
@@ -1457,7 +1445,7 @@
         <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
@@ -1550,11 +1538,11 @@
         <v>15</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N7">
         <f>COUNTIF(K2:K97,"&gt;0")</f>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
@@ -1584,7 +1572,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H8" s="7" t="str">
         <f>IF(F8="","", INDEX(Table4[],MATCH(F8,Table4[primer],0),1))</f>
@@ -1602,11 +1590,11 @@
         <v>15</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N8">
         <f>N7*5.5*1.1</f>
-        <v>108.9</v>
+        <v>157.30000000000001</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
@@ -1636,7 +1624,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H9" s="7" t="str">
         <f>IF(F9="","", INDEX(Table4[],MATCH(F9,Table4[primer],0),1))</f>
@@ -1752,20 +1740,23 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
+      <c r="F12" t="s">
+        <v>105</v>
+      </c>
       <c r="H12" s="7" t="str">
         <f>IF(F12="","", INDEX(Table4[],MATCH(F12,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I12" s="7" cm="1">
         <f t="array" ref="I12">_xlfn.IFS(F12="",0,F12="water",11.5, TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="P12">
         <f t="shared" si="0"/>
@@ -2334,6 +2325,12 @@
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
       <c r="H26" s="7" t="str">
         <f>IF(F26="","", INDEX(Table4[],MATCH(F26,Table4[primer],0),1))</f>
         <v/>
@@ -2347,11 +2344,11 @@
       </c>
       <c r="K26" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26">
         <f t="shared" si="3"/>
@@ -2359,7 +2356,7 @@
       </c>
       <c r="R26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T26" t="s">
         <v>27</v>
@@ -2370,6 +2367,12 @@
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
       <c r="H27" s="7" t="str">
         <f>IF(F27="","", INDEX(Table4[],MATCH(F27,Table4[primer],0),1))</f>
         <v/>
@@ -2383,11 +2386,11 @@
       </c>
       <c r="K27" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q27">
         <f t="shared" si="3"/>
@@ -2395,7 +2398,7 @@
       </c>
       <c r="R27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T27" t="s">
         <v>28</v>
@@ -2406,6 +2409,12 @@
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
       <c r="H28" s="7" t="str">
         <f>IF(F28="","", INDEX(Table4[],MATCH(F28,Table4[primer],0),1))</f>
         <v/>
@@ -2419,11 +2428,11 @@
       </c>
       <c r="K28" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28">
         <f t="shared" si="3"/>
@@ -2431,7 +2440,7 @@
       </c>
       <c r="R28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T28" t="s">
         <v>29</v>
@@ -2442,6 +2451,12 @@
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
       <c r="H29" s="7" t="str">
         <f>IF(F29="","", INDEX(Table4[],MATCH(F29,Table4[primer],0),1))</f>
         <v/>
@@ -2455,11 +2470,11 @@
       </c>
       <c r="K29" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29">
         <f t="shared" si="3"/>
@@ -2467,7 +2482,7 @@
       </c>
       <c r="R29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T29" t="s">
         <v>30</v>
@@ -2478,6 +2493,12 @@
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
       <c r="H30" s="7" t="str">
         <f>IF(F30="","", INDEX(Table4[],MATCH(F30,Table4[primer],0),1))</f>
         <v/>
@@ -2491,11 +2512,11 @@
       </c>
       <c r="K30" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30">
         <f t="shared" si="3"/>
@@ -2503,7 +2524,7 @@
       </c>
       <c r="R30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T30" t="s">
         <v>31</v>
@@ -2514,6 +2535,12 @@
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
       <c r="H31" s="7" t="str">
         <f>IF(F31="","", INDEX(Table4[],MATCH(F31,Table4[primer],0),1))</f>
         <v/>
@@ -2527,11 +2554,11 @@
       </c>
       <c r="K31" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q31">
         <f t="shared" si="3"/>
@@ -2539,7 +2566,7 @@
       </c>
       <c r="R31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T31" t="s">
         <v>32</v>
@@ -2550,6 +2577,12 @@
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
       <c r="H32" s="7" t="str">
         <f>IF(F32="","", INDEX(Table4[],MATCH(F32,Table4[primer],0),1))</f>
         <v/>
@@ -2563,11 +2596,11 @@
       </c>
       <c r="K32" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32">
         <f t="shared" si="3"/>
@@ -2575,7 +2608,7 @@
       </c>
       <c r="R32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T32" t="s">
         <v>33</v>
@@ -2585,7 +2618,13 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
       <c r="H33" s="7" t="str">
         <f>IF(F33="","", INDEX(Table4[],MATCH(F33,Table4[primer],0),1))</f>
         <v/>
@@ -2599,11 +2638,11 @@
       </c>
       <c r="K33" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q33">
         <f t="shared" si="3"/>
@@ -2611,7 +2650,7 @@
       </c>
       <c r="R33">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T33" t="s">
         <v>34</v>
@@ -2621,7 +2660,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H34" s="7" t="str">
         <f>IF(F34="","", INDEX(Table4[],MATCH(F34,Table4[primer],0),1))</f>
         <v/>
@@ -2657,7 +2696,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H35" s="7" t="str">
         <f>IF(F35="","", INDEX(Table4[],MATCH(F35,Table4[primer],0),1))</f>
         <v/>
@@ -2693,7 +2732,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H36" s="7" t="str">
         <f>IF(F36="","", INDEX(Table4[],MATCH(F36,Table4[primer],0),1))</f>
         <v/>
@@ -2729,7 +2768,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H37" s="7" t="str">
         <f>IF(F37="","", INDEX(Table4[],MATCH(F37,Table4[primer],0),1))</f>
         <v/>
@@ -2765,7 +2804,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H38" s="7" t="str">
         <f>IF(F38="","", INDEX(Table4[],MATCH(F38,Table4[primer],0),1))</f>
         <v/>
@@ -2801,7 +2840,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H39" s="7" t="str">
         <f>IF(F39="","", INDEX(Table4[],MATCH(F39,Table4[primer],0),1))</f>
         <v/>
@@ -2837,7 +2876,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H40" s="7" t="str">
         <f>IF(F40="","", INDEX(Table4[],MATCH(F40,Table4[primer],0),1))</f>
         <v/>
@@ -2873,7 +2912,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H41" s="7" t="str">
         <f>IF(F41="","", INDEX(Table4[],MATCH(F41,Table4[primer],0),1))</f>
         <v/>
@@ -2909,7 +2948,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H42" s="7" t="str">
         <f>IF(F42="","", INDEX(Table4[],MATCH(F42,Table4[primer],0),1))</f>
         <v/>
@@ -2945,7 +2984,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H43" s="7" t="str">
         <f>IF(F43="","", INDEX(Table4[],MATCH(F43,Table4[primer],0),1))</f>
         <v/>
@@ -2981,7 +3020,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H44" s="7" t="str">
         <f>IF(F44="","", INDEX(Table4[],MATCH(F44,Table4[primer],0),1))</f>
         <v/>
@@ -3017,7 +3056,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H45" s="7" t="str">
         <f>IF(F45="","", INDEX(Table4[],MATCH(F45,Table4[primer],0),1))</f>
         <v/>
@@ -3053,7 +3092,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H46" s="7" t="str">
         <f>IF(F46="","", INDEX(Table4[],MATCH(F46,Table4[primer],0),1))</f>
         <v/>
@@ -3089,7 +3128,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H47" s="7" t="str">
         <f>IF(F47="","", INDEX(Table4[],MATCH(F47,Table4[primer],0),1))</f>
         <v/>
@@ -3125,7 +3164,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
       <c r="H48" s="7" t="str">
         <f>IF(F48="","", INDEX(Table4[],MATCH(F48,Table4[primer],0),1))</f>
         <v/>
@@ -5011,7 +5050,7 @@
         <v>157</v>
       </c>
       <c r="J1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -5291,7 +5330,7 @@
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F21" t="s">
         <v>141</v>
@@ -5338,10 +5377,10 @@
         <v>46</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F25" t="s">
         <v>145</v>
@@ -5432,7 +5471,7 @@
     </row>
     <row r="36" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J36" t="s">
         <v>37</v>
@@ -5440,7 +5479,7 @@
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J37" t="s">
         <v>38</v>
@@ -6102,105 +6141,105 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
         <f>IF(master!B26="plate",master!C26, "")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="1">
         <f>IF(master!B26="plate",master!K26,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="str">
         <f>IF(master!B27="plate",master!C27, "")</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="1">
         <f>IF(master!B27="plate",master!K27,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="str">
         <f>IF(master!B28="plate",master!C28, "")</f>
-        <v/>
+        <v>C01</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="1">
         <f>IF(master!B28="plate",master!K28,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="str">
         <f>IF(master!B29="plate",master!C29, "")</f>
-        <v/>
+        <v>D01</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="1">
         <f>IF(master!B29="plate",master!K29,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="str">
         <f>IF(master!B30="plate",master!C30, "")</f>
-        <v/>
+        <v>E01</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="1">
         <f>IF(master!B30="plate",master!K30,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="str">
         <f>IF(master!B31="plate",master!C31, "")</f>
-        <v/>
+        <v>F01</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="1">
         <f>IF(master!B31="plate",master!K31,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="str">
         <f>IF(master!B32="plate",master!C32, "")</f>
-        <v/>
+        <v>G01</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="1">
         <f>IF(master!B32="plate",master!K32,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="str">
         <f>IF(master!B33="plate",master!C33, "")</f>
-        <v/>
+        <v>H01</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="1">
         <f>IF(master!B33="plate",master!K33,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -7214,7 +7253,7 @@
       </c>
       <c r="C12" s="1">
         <f>IF(master!B12="strip",master!K12,0)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -8496,14 +8535,14 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>IF(ISTEXT(master!F12),master!H12,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <f>master!I12</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -9629,7 +9668,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9641,31 +9680,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" t="s">
         <v>174</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>175</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>176</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>177</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>178</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>179</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>180</v>
-      </c>
-      <c r="H1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -10071,11 +10110,11 @@
       </c>
       <c r="F12">
         <f>source_strip!C12</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G12" t="str">
         <f>source_tube!A12</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H12" t="str">
         <f>source_tube!B12</f>
@@ -10083,7 +10122,7 @@
       </c>
       <c r="I12">
         <f>source_tube!C12</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -10583,7 +10622,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>source_plate!A26</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B26" t="str">
         <f>source_plate!B26</f>
@@ -10591,7 +10630,7 @@
       </c>
       <c r="C26">
         <f>source_plate!C26</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D26" t="str">
         <f>source_strip!A26</f>
@@ -10621,7 +10660,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>source_plate!A27</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B27" t="str">
         <f>source_plate!B27</f>
@@ -10629,7 +10668,7 @@
       </c>
       <c r="C27">
         <f>source_plate!C27</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D27" t="str">
         <f>source_strip!A27</f>
@@ -10659,7 +10698,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>source_plate!A28</f>
-        <v/>
+        <v>C01</v>
       </c>
       <c r="B28" t="str">
         <f>source_plate!B28</f>
@@ -10667,7 +10706,7 @@
       </c>
       <c r="C28">
         <f>source_plate!C28</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D28" t="str">
         <f>source_strip!A28</f>
@@ -10697,7 +10736,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>source_plate!A29</f>
-        <v/>
+        <v>D01</v>
       </c>
       <c r="B29" t="str">
         <f>source_plate!B29</f>
@@ -10705,7 +10744,7 @@
       </c>
       <c r="C29">
         <f>source_plate!C29</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D29" t="str">
         <f>source_strip!A29</f>
@@ -10735,7 +10774,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>source_plate!A30</f>
-        <v/>
+        <v>E01</v>
       </c>
       <c r="B30" t="str">
         <f>source_plate!B30</f>
@@ -10743,7 +10782,7 @@
       </c>
       <c r="C30">
         <f>source_plate!C30</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D30" t="str">
         <f>source_strip!A30</f>
@@ -10773,7 +10812,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>source_plate!A31</f>
-        <v/>
+        <v>F01</v>
       </c>
       <c r="B31" t="str">
         <f>source_plate!B31</f>
@@ -10781,7 +10820,7 @@
       </c>
       <c r="C31">
         <f>source_plate!C31</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D31" t="str">
         <f>source_strip!A31</f>
@@ -10811,7 +10850,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>source_plate!A32</f>
-        <v/>
+        <v>G01</v>
       </c>
       <c r="B32" t="str">
         <f>source_plate!B32</f>
@@ -10819,7 +10858,7 @@
       </c>
       <c r="C32">
         <f>source_plate!C32</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D32" t="str">
         <f>source_strip!A32</f>
@@ -10849,7 +10888,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>source_plate!A33</f>
-        <v/>
+        <v>H01</v>
       </c>
       <c r="B33" t="str">
         <f>source_plate!B33</f>
@@ -10857,7 +10896,7 @@
       </c>
       <c r="C33">
         <f>source_plate!C33</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D33" t="str">
         <f>source_strip!A33</f>

</xml_diff>

<commit_message>
add new ont plasmid seq protocol
</commit_message>
<xml_diff>
--- a/templates/01-sanger-master-v3.xlsx
+++ b/templates/01-sanger-master-v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60CC1C-A6F1-8C4C-B0BF-CEE2C9FA4294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA117C2-A7F2-AF43-8CA1-1D720A45CED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="760" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="193">
   <si>
     <t>source_well</t>
   </si>
@@ -779,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -799,7 +799,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1211,7 +1210,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1332,7 @@
       <c r="T2" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="19" t="str">
+      <c r="U2" t="str">
         <f>IF(ISBLANK(D2),"",D2)</f>
         <v>bla</v>
       </c>
@@ -1381,7 +1380,7 @@
       <c r="T3" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="19" t="str">
+      <c r="U3" t="str">
         <f t="shared" ref="U3:U66" si="4">IF(ISBLANK(D3),"",D3)</f>
         <v>1</v>
       </c>
@@ -1429,7 +1428,7 @@
       <c r="T4" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="19" t="str">
+      <c r="U4" t="str">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
@@ -1477,7 +1476,7 @@
       <c r="T5" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="19" t="str">
+      <c r="U5" t="str">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -1514,7 +1513,7 @@
       <c r="T6" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="19" t="str">
+      <c r="U6" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1541,7 +1540,7 @@
       </c>
       <c r="N7">
         <f>COUNTIF(K2:K97,"&gt;0")</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
@@ -1558,7 +1557,7 @@
       <c r="T7" t="s">
         <v>8</v>
       </c>
-      <c r="U7" s="19" t="str">
+      <c r="U7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1585,7 +1584,7 @@
       </c>
       <c r="N8">
         <f>N7*5.5*1.1</f>
-        <v>42.35</v>
+        <v>90.750000000000014</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
@@ -1602,31 +1601,40 @@
       <c r="T8" t="s">
         <v>9</v>
       </c>
-      <c r="U8" s="19" t="str">
+      <c r="U8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
       <c r="D9" s="17"/>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
       <c r="H9" s="7" t="str">
         <f>IF(F9="","", INDEX(Table4[],MATCH(F9,Table4[primer],0),1))</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="I9" s="7" cm="1">
         <f t="array" ref="I9">_xlfn.IFS(F9="",0,F9="water",11.5,TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="3"/>
@@ -1634,36 +1642,45 @@
       </c>
       <c r="R9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T9" t="s">
         <v>10</v>
       </c>
-      <c r="U9" s="19" t="str">
+      <c r="U9" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="17"/>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
       <c r="H10" s="7" t="str">
         <f>IF(F10="","", INDEX(Table4[],MATCH(F10,Table4[primer],0),1))</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="I10" s="7" cm="1">
         <f t="array" ref="I10">_xlfn.IFS(F10="",0,F10="water",11.5,TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f t="shared" si="3"/>
@@ -1671,36 +1688,45 @@
       </c>
       <c r="R10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T10" t="s">
         <v>11</v>
       </c>
-      <c r="U10" s="19" t="str">
+      <c r="U10" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
       <c r="D11" s="17"/>
+      <c r="F11" t="s">
+        <v>106</v>
+      </c>
       <c r="H11" s="7" t="str">
         <f>IF(F11="","", INDEX(Table4[],MATCH(F11,Table4[primer],0),1))</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="I11" s="7" cm="1">
         <f t="array" ref="I11">_xlfn.IFS(F11="",0,F11="water",11.5,TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <f t="shared" si="3"/>
@@ -1708,36 +1734,45 @@
       </c>
       <c r="R11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T11" t="s">
         <v>12</v>
       </c>
-      <c r="U11" s="19" t="str">
+      <c r="U11" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
       <c r="D12" s="17"/>
+      <c r="F12" t="s">
+        <v>106</v>
+      </c>
       <c r="H12" s="7" t="str">
         <f>IF(F12="","", INDEX(Table4[],MATCH(F12,Table4[primer],0),1))</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="I12" s="7" cm="1">
         <f t="array" ref="I12">_xlfn.IFS(F12="",0,F12="water",11.5,TRUE, 5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <f t="shared" si="3"/>
@@ -1745,12 +1780,12 @@
       </c>
       <c r="R12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T12" t="s">
         <v>13</v>
       </c>
-      <c r="U12" s="19" t="str">
+      <c r="U12" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1787,7 +1822,7 @@
       <c r="T13" t="s">
         <v>14</v>
       </c>
-      <c r="U13" s="19" t="str">
+      <c r="U13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1824,7 +1859,7 @@
       <c r="T14" t="s">
         <v>15</v>
       </c>
-      <c r="U14" s="19" t="str">
+      <c r="U14" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1861,7 +1896,7 @@
       <c r="T15" t="s">
         <v>16</v>
       </c>
-      <c r="U15" s="19" t="str">
+      <c r="U15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1898,12 +1933,12 @@
       <c r="T16" t="s">
         <v>17</v>
       </c>
-      <c r="U16" s="19" t="str">
+      <c r="U16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D17" s="17"/>
       <c r="H17" s="7" t="str">
         <f>IF(F17="","", INDEX(Table4[],MATCH(F17,Table4[primer],0),1))</f>
@@ -1935,12 +1970,18 @@
       <c r="T17" t="s">
         <v>18</v>
       </c>
-      <c r="U17" s="19" t="str">
+      <c r="U17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
       <c r="D18" s="17"/>
       <c r="H18" s="7" t="str">
         <f>IF(F18="","", INDEX(Table4[],MATCH(F18,Table4[primer],0),1))</f>
@@ -1955,11 +1996,11 @@
       </c>
       <c r="K18" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18">
         <f t="shared" si="3"/>
@@ -1967,17 +2008,23 @@
       </c>
       <c r="R18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
       </c>
-      <c r="U18" s="19" t="str">
+      <c r="U18" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
       <c r="D19" s="17"/>
       <c r="H19" s="7" t="str">
         <f>IF(F19="","", INDEX(Table4[],MATCH(F19,Table4[primer],0),1))</f>
@@ -1992,11 +2039,11 @@
       </c>
       <c r="K19" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19">
         <f t="shared" si="3"/>
@@ -2004,17 +2051,23 @@
       </c>
       <c r="R19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T19" t="s">
         <v>20</v>
       </c>
-      <c r="U19" s="19" t="str">
+      <c r="U19" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
       <c r="D20" s="17"/>
       <c r="H20" s="7" t="str">
         <f>IF(F20="","", INDEX(Table4[],MATCH(F20,Table4[primer],0),1))</f>
@@ -2029,11 +2082,11 @@
       </c>
       <c r="K20" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20">
         <f t="shared" si="3"/>
@@ -2041,17 +2094,23 @@
       </c>
       <c r="R20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T20" t="s">
         <v>21</v>
       </c>
-      <c r="U20" s="19" t="str">
+      <c r="U20" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
       <c r="D21" s="17"/>
       <c r="H21" s="7" t="str">
         <f>IF(F21="","", INDEX(Table4[],MATCH(F21,Table4[primer],0),1))</f>
@@ -2066,11 +2125,11 @@
       </c>
       <c r="K21" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
         <f t="shared" si="3"/>
@@ -2078,17 +2137,17 @@
       </c>
       <c r="R21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T21" t="s">
         <v>22</v>
       </c>
-      <c r="U21" s="19" t="str">
+      <c r="U21" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D22" s="17"/>
       <c r="H22" s="7" t="str">
         <f>IF(F22="","", INDEX(Table4[],MATCH(F22,Table4[primer],0),1))</f>
@@ -2120,12 +2179,12 @@
       <c r="T22" t="s">
         <v>23</v>
       </c>
-      <c r="U22" s="19" t="str">
+      <c r="U22" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D23" s="17"/>
       <c r="H23" s="7" t="str">
         <f>IF(F23="","", INDEX(Table4[],MATCH(F23,Table4[primer],0),1))</f>
@@ -2157,12 +2216,12 @@
       <c r="T23" t="s">
         <v>24</v>
       </c>
-      <c r="U23" s="19" t="str">
+      <c r="U23" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D24" s="17"/>
       <c r="H24" s="7" t="str">
         <f>IF(F24="","", INDEX(Table4[],MATCH(F24,Table4[primer],0),1))</f>
@@ -2194,12 +2253,12 @@
       <c r="T24" t="s">
         <v>25</v>
       </c>
-      <c r="U24" s="19" t="str">
+      <c r="U24" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D25" s="17"/>
       <c r="H25" s="7" t="str">
         <f>IF(F25="","", INDEX(Table4[],MATCH(F25,Table4[primer],0),1))</f>
@@ -2231,12 +2290,12 @@
       <c r="T25" t="s">
         <v>26</v>
       </c>
-      <c r="U25" s="19" t="str">
+      <c r="U25" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D26" s="17"/>
       <c r="H26" s="7" t="str">
         <f>IF(F26="","", INDEX(Table4[],MATCH(F26,Table4[primer],0),1))</f>
@@ -2268,12 +2327,12 @@
       <c r="T26" t="s">
         <v>27</v>
       </c>
-      <c r="U26" s="19" t="str">
+      <c r="U26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D27" s="17"/>
       <c r="H27" s="7" t="str">
         <f>IF(F27="","", INDEX(Table4[],MATCH(F27,Table4[primer],0),1))</f>
@@ -2305,12 +2364,12 @@
       <c r="T27" t="s">
         <v>28</v>
       </c>
-      <c r="U27" s="19" t="str">
+      <c r="U27" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D28" s="17"/>
       <c r="H28" s="7" t="str">
         <f>IF(F28="","", INDEX(Table4[],MATCH(F28,Table4[primer],0),1))</f>
@@ -2342,12 +2401,12 @@
       <c r="T28" t="s">
         <v>29</v>
       </c>
-      <c r="U28" s="19" t="str">
+      <c r="U28" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D29" s="17"/>
       <c r="H29" s="7" t="str">
         <f>IF(F29="","", INDEX(Table4[],MATCH(F29,Table4[primer],0),1))</f>
@@ -2379,12 +2438,12 @@
       <c r="T29" t="s">
         <v>30</v>
       </c>
-      <c r="U29" s="19" t="str">
+      <c r="U29" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D30" s="17"/>
       <c r="H30" s="7" t="str">
         <f>IF(F30="","", INDEX(Table4[],MATCH(F30,Table4[primer],0),1))</f>
@@ -2416,12 +2475,12 @@
       <c r="T30" t="s">
         <v>31</v>
       </c>
-      <c r="U30" s="19" t="str">
+      <c r="U30" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D31" s="17"/>
       <c r="H31" s="7" t="str">
         <f>IF(F31="","", INDEX(Table4[],MATCH(F31,Table4[primer],0),1))</f>
@@ -2453,12 +2512,12 @@
       <c r="T31" t="s">
         <v>32</v>
       </c>
-      <c r="U31" s="19" t="str">
+      <c r="U31" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D32" s="17"/>
       <c r="H32" s="7" t="str">
         <f>IF(F32="","", INDEX(Table4[],MATCH(F32,Table4[primer],0),1))</f>
@@ -2490,7 +2549,7 @@
       <c r="T32" t="s">
         <v>33</v>
       </c>
-      <c r="U32" s="19" t="str">
+      <c r="U32" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2527,7 +2586,7 @@
       <c r="T33" t="s">
         <v>34</v>
       </c>
-      <c r="U33" s="19" t="str">
+      <c r="U33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2564,7 +2623,7 @@
       <c r="T34" t="s">
         <v>35</v>
       </c>
-      <c r="U34" s="19" t="str">
+      <c r="U34" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2601,7 +2660,7 @@
       <c r="T35" t="s">
         <v>36</v>
       </c>
-      <c r="U35" s="19" t="str">
+      <c r="U35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2638,7 +2697,7 @@
       <c r="T36" t="s">
         <v>37</v>
       </c>
-      <c r="U36" s="19" t="str">
+      <c r="U36" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2675,7 +2734,7 @@
       <c r="T37" t="s">
         <v>38</v>
       </c>
-      <c r="U37" s="19" t="str">
+      <c r="U37" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2712,7 +2771,7 @@
       <c r="T38" t="s">
         <v>39</v>
       </c>
-      <c r="U38" s="19" t="str">
+      <c r="U38" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2749,7 +2808,7 @@
       <c r="T39" t="s">
         <v>40</v>
       </c>
-      <c r="U39" s="19" t="str">
+      <c r="U39" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2786,7 +2845,7 @@
       <c r="T40" t="s">
         <v>41</v>
       </c>
-      <c r="U40" s="19" t="str">
+      <c r="U40" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2823,7 +2882,7 @@
       <c r="T41" t="s">
         <v>42</v>
       </c>
-      <c r="U41" s="19" t="str">
+      <c r="U41" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2860,7 +2919,7 @@
       <c r="T42" t="s">
         <v>43</v>
       </c>
-      <c r="U42" s="19" t="str">
+      <c r="U42" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2897,7 +2956,7 @@
       <c r="T43" t="s">
         <v>44</v>
       </c>
-      <c r="U43" s="19" t="str">
+      <c r="U43" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2934,7 +2993,7 @@
       <c r="T44" t="s">
         <v>45</v>
       </c>
-      <c r="U44" s="19" t="str">
+      <c r="U44" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2971,7 +3030,7 @@
       <c r="T45" t="s">
         <v>46</v>
       </c>
-      <c r="U45" s="19" t="str">
+      <c r="U45" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3008,7 +3067,7 @@
       <c r="T46" t="s">
         <v>47</v>
       </c>
-      <c r="U46" s="19" t="str">
+      <c r="U46" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3045,7 +3104,7 @@
       <c r="T47" t="s">
         <v>48</v>
       </c>
-      <c r="U47" s="19" t="str">
+      <c r="U47" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3082,7 +3141,7 @@
       <c r="T48" t="s">
         <v>49</v>
       </c>
-      <c r="U48" s="19" t="str">
+      <c r="U48" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3119,7 +3178,7 @@
       <c r="T49" t="s">
         <v>50</v>
       </c>
-      <c r="U49" s="19" t="str">
+      <c r="U49" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3156,7 +3215,7 @@
       <c r="T50" t="s">
         <v>51</v>
       </c>
-      <c r="U50" s="19" t="str">
+      <c r="U50" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3193,7 +3252,7 @@
       <c r="T51" t="s">
         <v>52</v>
       </c>
-      <c r="U51" s="19" t="str">
+      <c r="U51" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3230,7 +3289,7 @@
       <c r="T52" t="s">
         <v>53</v>
       </c>
-      <c r="U52" s="19" t="str">
+      <c r="U52" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3267,7 +3326,7 @@
       <c r="T53" t="s">
         <v>54</v>
       </c>
-      <c r="U53" s="19" t="str">
+      <c r="U53" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3304,7 +3363,7 @@
       <c r="T54" t="s">
         <v>55</v>
       </c>
-      <c r="U54" s="19" t="str">
+      <c r="U54" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3341,7 +3400,7 @@
       <c r="T55" t="s">
         <v>56</v>
       </c>
-      <c r="U55" s="19" t="str">
+      <c r="U55" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3378,7 +3437,7 @@
       <c r="T56" t="s">
         <v>57</v>
       </c>
-      <c r="U56" s="19" t="str">
+      <c r="U56" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3415,7 +3474,7 @@
       <c r="T57" t="s">
         <v>58</v>
       </c>
-      <c r="U57" s="19" t="str">
+      <c r="U57" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3452,7 +3511,7 @@
       <c r="T58" t="s">
         <v>59</v>
       </c>
-      <c r="U58" s="19" t="str">
+      <c r="U58" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3489,7 +3548,7 @@
       <c r="T59" t="s">
         <v>60</v>
       </c>
-      <c r="U59" s="19" t="str">
+      <c r="U59" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3526,7 +3585,7 @@
       <c r="T60" t="s">
         <v>61</v>
       </c>
-      <c r="U60" s="19" t="str">
+      <c r="U60" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3563,7 +3622,7 @@
       <c r="T61" t="s">
         <v>62</v>
       </c>
-      <c r="U61" s="19" t="str">
+      <c r="U61" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3600,7 +3659,7 @@
       <c r="T62" t="s">
         <v>63</v>
       </c>
-      <c r="U62" s="19" t="str">
+      <c r="U62" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3637,7 +3696,7 @@
       <c r="T63" t="s">
         <v>64</v>
       </c>
-      <c r="U63" s="19" t="str">
+      <c r="U63" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3674,7 +3733,7 @@
       <c r="T64" t="s">
         <v>65</v>
       </c>
-      <c r="U64" s="19" t="str">
+      <c r="U64" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3711,7 +3770,7 @@
       <c r="T65" t="s">
         <v>66</v>
       </c>
-      <c r="U65" s="19" t="str">
+      <c r="U65" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3748,7 +3807,7 @@
       <c r="T66" t="s">
         <v>67</v>
       </c>
-      <c r="U66" s="19" t="str">
+      <c r="U66" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3785,7 +3844,7 @@
       <c r="T67" t="s">
         <v>68</v>
       </c>
-      <c r="U67" s="19" t="str">
+      <c r="U67" t="str">
         <f t="shared" ref="U67:U97" si="11">IF(ISBLANK(D67),"",D67)</f>
         <v/>
       </c>
@@ -3822,7 +3881,7 @@
       <c r="T68" t="s">
         <v>69</v>
       </c>
-      <c r="U68" s="19" t="str">
+      <c r="U68" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -3859,7 +3918,7 @@
       <c r="T69" t="s">
         <v>70</v>
       </c>
-      <c r="U69" s="19" t="str">
+      <c r="U69" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -3896,7 +3955,7 @@
       <c r="T70" t="s">
         <v>71</v>
       </c>
-      <c r="U70" s="19" t="str">
+      <c r="U70" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -3933,7 +3992,7 @@
       <c r="T71" t="s">
         <v>72</v>
       </c>
-      <c r="U71" s="19" t="str">
+      <c r="U71" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -3970,7 +4029,7 @@
       <c r="T72" t="s">
         <v>73</v>
       </c>
-      <c r="U72" s="19" t="str">
+      <c r="U72" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4007,7 +4066,7 @@
       <c r="T73" t="s">
         <v>74</v>
       </c>
-      <c r="U73" s="19" t="str">
+      <c r="U73" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4044,7 +4103,7 @@
       <c r="T74" t="s">
         <v>75</v>
       </c>
-      <c r="U74" s="19" t="str">
+      <c r="U74" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4081,7 +4140,7 @@
       <c r="T75" t="s">
         <v>76</v>
       </c>
-      <c r="U75" s="19" t="str">
+      <c r="U75" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4118,7 +4177,7 @@
       <c r="T76" t="s">
         <v>77</v>
       </c>
-      <c r="U76" s="19" t="str">
+      <c r="U76" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4155,7 +4214,7 @@
       <c r="T77" t="s">
         <v>78</v>
       </c>
-      <c r="U77" s="19" t="str">
+      <c r="U77" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4192,7 +4251,7 @@
       <c r="T78" t="s">
         <v>79</v>
       </c>
-      <c r="U78" s="19" t="str">
+      <c r="U78" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4229,7 +4288,7 @@
       <c r="T79" t="s">
         <v>80</v>
       </c>
-      <c r="U79" s="19" t="str">
+      <c r="U79" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4266,7 +4325,7 @@
       <c r="T80" t="s">
         <v>81</v>
       </c>
-      <c r="U80" s="19" t="str">
+      <c r="U80" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4303,7 +4362,7 @@
       <c r="T81" t="s">
         <v>82</v>
       </c>
-      <c r="U81" s="19" t="str">
+      <c r="U81" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4340,7 +4399,7 @@
       <c r="T82" t="s">
         <v>83</v>
       </c>
-      <c r="U82" s="19" t="str">
+      <c r="U82" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4377,7 +4436,7 @@
       <c r="T83" t="s">
         <v>84</v>
       </c>
-      <c r="U83" s="19" t="str">
+      <c r="U83" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4414,7 +4473,7 @@
       <c r="T84" t="s">
         <v>85</v>
       </c>
-      <c r="U84" s="19" t="str">
+      <c r="U84" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4451,7 +4510,7 @@
       <c r="T85" t="s">
         <v>86</v>
       </c>
-      <c r="U85" s="19" t="str">
+      <c r="U85" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4488,7 +4547,7 @@
       <c r="T86" t="s">
         <v>87</v>
       </c>
-      <c r="U86" s="19" t="str">
+      <c r="U86" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4525,7 +4584,7 @@
       <c r="T87" t="s">
         <v>88</v>
       </c>
-      <c r="U87" s="19" t="str">
+      <c r="U87" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4562,7 +4621,7 @@
       <c r="T88" t="s">
         <v>89</v>
       </c>
-      <c r="U88" s="19" t="str">
+      <c r="U88" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4599,7 +4658,7 @@
       <c r="T89" t="s">
         <v>90</v>
       </c>
-      <c r="U89" s="19" t="str">
+      <c r="U89" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4636,7 +4695,7 @@
       <c r="T90" t="s">
         <v>91</v>
       </c>
-      <c r="U90" s="19" t="str">
+      <c r="U90" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4673,7 +4732,7 @@
       <c r="T91" t="s">
         <v>92</v>
       </c>
-      <c r="U91" s="19" t="str">
+      <c r="U91" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4710,7 +4769,7 @@
       <c r="T92" t="s">
         <v>93</v>
       </c>
-      <c r="U92" s="19" t="str">
+      <c r="U92" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4747,7 +4806,7 @@
       <c r="T93" t="s">
         <v>94</v>
       </c>
-      <c r="U93" s="19" t="str">
+      <c r="U93" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4784,7 +4843,7 @@
       <c r="T94" t="s">
         <v>95</v>
       </c>
-      <c r="U94" s="19" t="str">
+      <c r="U94" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -4829,7 +4888,7 @@
       <c r="T95" t="s">
         <v>96</v>
       </c>
-      <c r="U95" s="19" t="str">
+      <c r="U95" t="str">
         <f t="shared" si="11"/>
         <v>Positive control</v>
       </c>
@@ -4874,7 +4933,7 @@
       <c r="T96" t="s">
         <v>97</v>
       </c>
-      <c r="U96" s="19" t="str">
+      <c r="U96" t="str">
         <f t="shared" si="11"/>
         <v>Positive control</v>
       </c>
@@ -4919,7 +4978,7 @@
       <c r="T97" t="s">
         <v>98</v>
       </c>
-      <c r="U97" s="19" t="str">
+      <c r="U97" t="str">
         <f t="shared" si="11"/>
         <v>Positive control</v>
       </c>
@@ -4984,8 +5043,8 @@
   </sheetPr>
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5770,7 +5829,7 @@
   <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7054,7 +7113,7 @@
   <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A18" sqref="A18:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7167,53 +7226,53 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>IF(master!B9="strip",master!C9,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1">
         <f>IF(master!B9="strip",master!K9,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>IF(master!B10="strip",master!C10,"")</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1">
         <f>IF(master!B10="strip",master!K10,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f>IF(master!B11="strip",master!C11,"")</f>
-        <v/>
+        <v>C01</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
         <f>IF(master!B11="strip",master!K11,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>IF(master!B12="strip",master!C12,"")</f>
-        <v/>
+        <v>D01</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <f>IF(master!B12="strip",master!K12,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -7284,53 +7343,53 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(master!B18="strip",master!C18,"")</f>
-        <v/>
+        <v>A02</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1">
         <f>IF(master!B18="strip",master!K18,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f>IF(master!B19="strip",master!C19,"")</f>
-        <v/>
+        <v>B02</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1">
         <f>IF(master!B19="strip",master!K19,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f>IF(master!B20="strip",master!C20,"")</f>
-        <v/>
+        <v>C02</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="1">
         <f>IF(master!B20="strip",master!K20,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f>IF(master!B21="strip",master!C21,"")</f>
-        <v/>
+        <v>D02</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="1">
         <f>IF(master!B21="strip",master!K21,0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -8341,7 +8400,7 @@
   <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A9" sqref="A9:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8456,53 +8515,53 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>IF(ISTEXT(master!F9),master!H9,"")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1">
         <f>master!I9</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>IF(ISTEXT(master!F10),master!H10,"")</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1">
         <f>master!I10</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f>IF(ISTEXT(master!F11),master!H11,"")</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
         <f>master!I11</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>IF(ISTEXT(master!F12),master!H12,"")</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <f>master!I12</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -9628,7 +9687,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9948,7 +10007,7 @@
       </c>
       <c r="D9" t="str">
         <f>source_strip!A9</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="E9" t="str">
         <f>source_strip!B9</f>
@@ -9956,11 +10015,11 @@
       </c>
       <c r="F9">
         <f>source_strip!C9</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G9" t="str">
         <f>source_tube!A9</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="H9" t="str">
         <f>source_tube!B9</f>
@@ -9968,7 +10027,7 @@
       </c>
       <c r="I9">
         <f>source_tube!C9</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -9986,7 +10045,7 @@
       </c>
       <c r="D10" t="str">
         <f>source_strip!A10</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="E10" t="str">
         <f>source_strip!B10</f>
@@ -9994,11 +10053,11 @@
       </c>
       <c r="F10">
         <f>source_strip!C10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G10" t="str">
         <f>source_tube!A10</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="H10" t="str">
         <f>source_tube!B10</f>
@@ -10006,7 +10065,7 @@
       </c>
       <c r="I10">
         <f>source_tube!C10</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -10024,7 +10083,7 @@
       </c>
       <c r="D11" t="str">
         <f>source_strip!A11</f>
-        <v/>
+        <v>C01</v>
       </c>
       <c r="E11" t="str">
         <f>source_strip!B11</f>
@@ -10032,11 +10091,11 @@
       </c>
       <c r="F11">
         <f>source_strip!C11</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G11" t="str">
         <f>source_tube!A11</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="H11" t="str">
         <f>source_tube!B11</f>
@@ -10044,7 +10103,7 @@
       </c>
       <c r="I11">
         <f>source_tube!C11</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -10062,7 +10121,7 @@
       </c>
       <c r="D12" t="str">
         <f>source_strip!A12</f>
-        <v/>
+        <v>D01</v>
       </c>
       <c r="E12" t="str">
         <f>source_strip!B12</f>
@@ -10070,11 +10129,11 @@
       </c>
       <c r="F12">
         <f>source_strip!C12</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G12" t="str">
         <f>source_tube!A12</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="H12" t="str">
         <f>source_tube!B12</f>
@@ -10082,7 +10141,7 @@
       </c>
       <c r="I12">
         <f>source_tube!C12</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -10290,7 +10349,7 @@
       </c>
       <c r="D18" t="str">
         <f>source_strip!A18</f>
-        <v/>
+        <v>A02</v>
       </c>
       <c r="E18" t="str">
         <f>source_strip!B18</f>
@@ -10298,7 +10357,7 @@
       </c>
       <c r="F18">
         <f>source_strip!C18</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G18" t="str">
         <f>source_tube!A18</f>
@@ -10328,7 +10387,7 @@
       </c>
       <c r="D19" t="str">
         <f>source_strip!A19</f>
-        <v/>
+        <v>B02</v>
       </c>
       <c r="E19" t="str">
         <f>source_strip!B19</f>
@@ -10336,7 +10395,7 @@
       </c>
       <c r="F19">
         <f>source_strip!C19</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G19" t="str">
         <f>source_tube!A19</f>
@@ -10366,7 +10425,7 @@
       </c>
       <c r="D20" t="str">
         <f>source_strip!A20</f>
-        <v/>
+        <v>C02</v>
       </c>
       <c r="E20" t="str">
         <f>source_strip!B20</f>
@@ -10374,7 +10433,7 @@
       </c>
       <c r="F20">
         <f>source_strip!C20</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G20" t="str">
         <f>source_tube!A20</f>
@@ -10404,7 +10463,7 @@
       </c>
       <c r="D21" t="str">
         <f>source_strip!A21</f>
-        <v/>
+        <v>D02</v>
       </c>
       <c r="E21" t="str">
         <f>source_strip!B21</f>
@@ -10412,7 +10471,7 @@
       </c>
       <c r="F21">
         <f>source_strip!C21</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G21" t="str">
         <f>source_tube!A21</f>
@@ -13331,6 +13390,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FDAF843F15E65A4EA1FFB0CF193B74E3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd4433bf6f24a726161ac457e21002bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1a61fc9-c776-4dd1-85b5-f7d58768ba79" xmlns:ns4="3f421247-72bc-4b61-a591-0b56f96ae993" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d66d7a13b7b51360e8b1c095fb39c19" ns3:_="" ns4:_="">
     <xsd:import namespace="e1a61fc9-c776-4dd1-85b5-f7d58768ba79"/>
@@ -13559,12 +13624,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79D86924-57C1-45D5-9E44-D526494DB02F}">
   <ds:schemaRefs>
@@ -13574,6 +13633,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CD12B7-1FA3-4B61-BDAE-DF4259CEDD3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3f421247-72bc-4b61-a591-0b56f96ae993"/>
+    <ds:schemaRef ds:uri="e1a61fc9-c776-4dd1-85b5-f7d58768ba79"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E774FF9-2144-4DC7-8F36-E7E064C7C739}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13590,21 +13666,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CD12B7-1FA3-4B61-BDAE-DF4259CEDD3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3f421247-72bc-4b61-a591-0b56f96ae993"/>
-    <ds:schemaRef ds:uri="e1a61fc9-c776-4dd1-85b5-f7d58768ba79"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>